<commit_message>
suppression assay tb 10/04
</commit_message>
<xml_diff>
--- a/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
+++ b/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiabrown/Documents/git/cest-2.1-Project/Tia_Jub39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C592375-31C1-D145-B0C1-DEB91ECC528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B1FDD6-AC00-E54C-88F0-4C75B2169D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15600" xr2:uid="{DD7AC6D9-FEFD-0E41-A755-99DADF736280}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="14">
   <si>
     <t>100pct</t>
   </si>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A9CC03-DE84-E245-89A8-02F35FB81FD2}">
-  <dimension ref="A1:F632"/>
+  <dimension ref="A1:F715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A551" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G571" sqref="G571"/>
+    <sheetView tabSelected="1" topLeftCell="A681" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G704" sqref="G704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13096,6 +13096,1666 @@
         <v>44831</v>
       </c>
     </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A633" t="s">
+        <v>2</v>
+      </c>
+      <c r="B633" t="s">
+        <v>11</v>
+      </c>
+      <c r="C633" t="s">
+        <v>0</v>
+      </c>
+      <c r="D633" s="2">
+        <v>6.55</v>
+      </c>
+      <c r="E633" t="s">
+        <v>1</v>
+      </c>
+      <c r="F633" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>2</v>
+      </c>
+      <c r="B634" t="s">
+        <v>11</v>
+      </c>
+      <c r="C634" t="s">
+        <v>0</v>
+      </c>
+      <c r="D634">
+        <v>2.98</v>
+      </c>
+      <c r="E634" t="s">
+        <v>1</v>
+      </c>
+      <c r="F634" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>2</v>
+      </c>
+      <c r="B635" t="s">
+        <v>11</v>
+      </c>
+      <c r="C635" t="s">
+        <v>0</v>
+      </c>
+      <c r="D635">
+        <v>4.93</v>
+      </c>
+      <c r="E635" t="s">
+        <v>1</v>
+      </c>
+      <c r="F635" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>2</v>
+      </c>
+      <c r="B636" t="s">
+        <v>11</v>
+      </c>
+      <c r="C636" t="s">
+        <v>0</v>
+      </c>
+      <c r="D636">
+        <v>3.28</v>
+      </c>
+      <c r="E636" t="s">
+        <v>1</v>
+      </c>
+      <c r="F636" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A637" t="s">
+        <v>2</v>
+      </c>
+      <c r="B637" t="s">
+        <v>11</v>
+      </c>
+      <c r="C637" t="s">
+        <v>0</v>
+      </c>
+      <c r="D637">
+        <v>6.98</v>
+      </c>
+      <c r="E637" t="s">
+        <v>1</v>
+      </c>
+      <c r="F637" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>2</v>
+      </c>
+      <c r="B638" t="s">
+        <v>11</v>
+      </c>
+      <c r="C638" t="s">
+        <v>0</v>
+      </c>
+      <c r="D638">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E638" t="s">
+        <v>1</v>
+      </c>
+      <c r="F638" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>2</v>
+      </c>
+      <c r="B639" t="s">
+        <v>11</v>
+      </c>
+      <c r="C639" t="s">
+        <v>0</v>
+      </c>
+      <c r="D639">
+        <v>3.52</v>
+      </c>
+      <c r="E639" t="s">
+        <v>1</v>
+      </c>
+      <c r="F639" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>2</v>
+      </c>
+      <c r="B640" t="s">
+        <v>11</v>
+      </c>
+      <c r="C640" t="s">
+        <v>0</v>
+      </c>
+      <c r="D640">
+        <v>6.98</v>
+      </c>
+      <c r="E640" t="s">
+        <v>1</v>
+      </c>
+      <c r="F640" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A641" t="s">
+        <v>2</v>
+      </c>
+      <c r="B641" t="s">
+        <v>11</v>
+      </c>
+      <c r="C641" t="s">
+        <v>0</v>
+      </c>
+      <c r="D641">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="E641" t="s">
+        <v>1</v>
+      </c>
+      <c r="F641" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A642" t="s">
+        <v>2</v>
+      </c>
+      <c r="B642" t="s">
+        <v>11</v>
+      </c>
+      <c r="C642" t="s">
+        <v>0</v>
+      </c>
+      <c r="D642">
+        <v>3.52</v>
+      </c>
+      <c r="E642" t="s">
+        <v>1</v>
+      </c>
+      <c r="F642" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A643" t="s">
+        <v>2</v>
+      </c>
+      <c r="B643" t="s">
+        <v>11</v>
+      </c>
+      <c r="C643" t="s">
+        <v>0</v>
+      </c>
+      <c r="D643">
+        <v>2.94</v>
+      </c>
+      <c r="E643" t="s">
+        <v>1</v>
+      </c>
+      <c r="F643" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A644" t="s">
+        <v>2</v>
+      </c>
+      <c r="B644" t="s">
+        <v>11</v>
+      </c>
+      <c r="C644" t="s">
+        <v>0</v>
+      </c>
+      <c r="D644">
+        <v>5.75</v>
+      </c>
+      <c r="E644" t="s">
+        <v>1</v>
+      </c>
+      <c r="F644" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A645" t="s">
+        <v>2</v>
+      </c>
+      <c r="B645" t="s">
+        <v>11</v>
+      </c>
+      <c r="C645" t="s">
+        <v>0</v>
+      </c>
+      <c r="D645">
+        <v>9.07</v>
+      </c>
+      <c r="E645" t="s">
+        <v>1</v>
+      </c>
+      <c r="F645" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>2</v>
+      </c>
+      <c r="B646" t="s">
+        <v>11</v>
+      </c>
+      <c r="C646" t="s">
+        <v>0</v>
+      </c>
+      <c r="D646">
+        <v>12.34</v>
+      </c>
+      <c r="E646" t="s">
+        <v>1</v>
+      </c>
+      <c r="F646" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>2</v>
+      </c>
+      <c r="B647" t="s">
+        <v>11</v>
+      </c>
+      <c r="C647" t="s">
+        <v>0</v>
+      </c>
+      <c r="D647">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="E647" t="s">
+        <v>1</v>
+      </c>
+      <c r="F647" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A648" t="s">
+        <v>2</v>
+      </c>
+      <c r="B648" t="s">
+        <v>11</v>
+      </c>
+      <c r="C648" t="s">
+        <v>0</v>
+      </c>
+      <c r="D648">
+        <v>9.16</v>
+      </c>
+      <c r="E648" t="s">
+        <v>1</v>
+      </c>
+      <c r="F648" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A649" t="s">
+        <v>2</v>
+      </c>
+      <c r="B649" t="s">
+        <v>11</v>
+      </c>
+      <c r="C649" t="s">
+        <v>0</v>
+      </c>
+      <c r="D649">
+        <v>13.01</v>
+      </c>
+      <c r="E649" t="s">
+        <v>1</v>
+      </c>
+      <c r="F649" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A650" t="s">
+        <v>2</v>
+      </c>
+      <c r="B650" t="s">
+        <v>11</v>
+      </c>
+      <c r="C650" t="s">
+        <v>0</v>
+      </c>
+      <c r="D650">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E650" t="s">
+        <v>1</v>
+      </c>
+      <c r="F650" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A651" t="s">
+        <v>2</v>
+      </c>
+      <c r="B651" t="s">
+        <v>11</v>
+      </c>
+      <c r="C651" t="s">
+        <v>0</v>
+      </c>
+      <c r="D651">
+        <v>3.23</v>
+      </c>
+      <c r="E651" t="s">
+        <v>1</v>
+      </c>
+      <c r="F651" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A652" t="s">
+        <v>2</v>
+      </c>
+      <c r="B652" t="s">
+        <v>11</v>
+      </c>
+      <c r="C652" t="s">
+        <v>0</v>
+      </c>
+      <c r="D652">
+        <v>3.49</v>
+      </c>
+      <c r="E652" t="s">
+        <v>1</v>
+      </c>
+      <c r="F652" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A653" t="s">
+        <v>2</v>
+      </c>
+      <c r="B653" t="s">
+        <v>11</v>
+      </c>
+      <c r="C653" t="s">
+        <v>0</v>
+      </c>
+      <c r="D653">
+        <v>4.25</v>
+      </c>
+      <c r="E653" t="s">
+        <v>1</v>
+      </c>
+      <c r="F653" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A654" t="s">
+        <v>2</v>
+      </c>
+      <c r="B654" t="s">
+        <v>11</v>
+      </c>
+      <c r="C654" t="s">
+        <v>0</v>
+      </c>
+      <c r="D654">
+        <v>3.86</v>
+      </c>
+      <c r="E654" t="s">
+        <v>1</v>
+      </c>
+      <c r="F654" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="655" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A655" t="s">
+        <v>2</v>
+      </c>
+      <c r="B655" t="s">
+        <v>11</v>
+      </c>
+      <c r="C655" t="s">
+        <v>0</v>
+      </c>
+      <c r="D655">
+        <v>11.75</v>
+      </c>
+      <c r="E655" t="s">
+        <v>1</v>
+      </c>
+      <c r="F655" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="656" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A656" t="s">
+        <v>10</v>
+      </c>
+      <c r="B656" t="s">
+        <v>11</v>
+      </c>
+      <c r="C656" t="s">
+        <v>0</v>
+      </c>
+      <c r="D656">
+        <v>16.14</v>
+      </c>
+      <c r="E656" t="s">
+        <v>1</v>
+      </c>
+      <c r="F656" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="657" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A657" t="s">
+        <v>10</v>
+      </c>
+      <c r="B657" t="s">
+        <v>11</v>
+      </c>
+      <c r="C657" t="s">
+        <v>0</v>
+      </c>
+      <c r="D657">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E657" t="s">
+        <v>1</v>
+      </c>
+      <c r="F657" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="658" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A658" t="s">
+        <v>10</v>
+      </c>
+      <c r="B658" t="s">
+        <v>11</v>
+      </c>
+      <c r="C658" t="s">
+        <v>0</v>
+      </c>
+      <c r="D658">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E658" t="s">
+        <v>1</v>
+      </c>
+      <c r="F658" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="659" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A659" t="s">
+        <v>10</v>
+      </c>
+      <c r="B659" t="s">
+        <v>11</v>
+      </c>
+      <c r="C659" t="s">
+        <v>0</v>
+      </c>
+      <c r="D659">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="E659" t="s">
+        <v>1</v>
+      </c>
+      <c r="F659" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="660" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A660" t="s">
+        <v>10</v>
+      </c>
+      <c r="B660" t="s">
+        <v>11</v>
+      </c>
+      <c r="C660" t="s">
+        <v>0</v>
+      </c>
+      <c r="D660">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="E660" t="s">
+        <v>1</v>
+      </c>
+      <c r="F660" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="661" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A661" t="s">
+        <v>10</v>
+      </c>
+      <c r="B661" t="s">
+        <v>11</v>
+      </c>
+      <c r="C661" t="s">
+        <v>0</v>
+      </c>
+      <c r="D661">
+        <v>3.96</v>
+      </c>
+      <c r="E661" t="s">
+        <v>1</v>
+      </c>
+      <c r="F661" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="662" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A662" t="s">
+        <v>10</v>
+      </c>
+      <c r="B662" t="s">
+        <v>11</v>
+      </c>
+      <c r="C662" t="s">
+        <v>0</v>
+      </c>
+      <c r="D662">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E662" t="s">
+        <v>1</v>
+      </c>
+      <c r="F662" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="663" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A663" t="s">
+        <v>10</v>
+      </c>
+      <c r="B663" t="s">
+        <v>11</v>
+      </c>
+      <c r="C663" t="s">
+        <v>0</v>
+      </c>
+      <c r="D663">
+        <v>6.78</v>
+      </c>
+      <c r="E663" t="s">
+        <v>1</v>
+      </c>
+      <c r="F663" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="664" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A664" t="s">
+        <v>10</v>
+      </c>
+      <c r="B664" t="s">
+        <v>11</v>
+      </c>
+      <c r="C664" t="s">
+        <v>0</v>
+      </c>
+      <c r="D664">
+        <v>4.22</v>
+      </c>
+      <c r="E664" t="s">
+        <v>1</v>
+      </c>
+      <c r="F664" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="665" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A665" t="s">
+        <v>10</v>
+      </c>
+      <c r="B665" t="s">
+        <v>11</v>
+      </c>
+      <c r="C665" t="s">
+        <v>0</v>
+      </c>
+      <c r="D665">
+        <v>4.82</v>
+      </c>
+      <c r="E665" t="s">
+        <v>1</v>
+      </c>
+      <c r="F665" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="666" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A666" t="s">
+        <v>10</v>
+      </c>
+      <c r="B666" t="s">
+        <v>11</v>
+      </c>
+      <c r="C666" t="s">
+        <v>0</v>
+      </c>
+      <c r="D666">
+        <v>5.53</v>
+      </c>
+      <c r="E666" t="s">
+        <v>1</v>
+      </c>
+      <c r="F666" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="667" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A667" t="s">
+        <v>10</v>
+      </c>
+      <c r="B667" t="s">
+        <v>11</v>
+      </c>
+      <c r="C667" t="s">
+        <v>0</v>
+      </c>
+      <c r="D667">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E667" t="s">
+        <v>1</v>
+      </c>
+      <c r="F667" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="668" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A668" t="s">
+        <v>10</v>
+      </c>
+      <c r="B668" t="s">
+        <v>11</v>
+      </c>
+      <c r="C668" t="s">
+        <v>0</v>
+      </c>
+      <c r="D668">
+        <v>2.62</v>
+      </c>
+      <c r="E668" t="s">
+        <v>1</v>
+      </c>
+      <c r="F668" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="669" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A669" t="s">
+        <v>10</v>
+      </c>
+      <c r="B669" t="s">
+        <v>11</v>
+      </c>
+      <c r="C669" t="s">
+        <v>0</v>
+      </c>
+      <c r="D669">
+        <v>3.3</v>
+      </c>
+      <c r="E669" t="s">
+        <v>1</v>
+      </c>
+      <c r="F669" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="670" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A670" t="s">
+        <v>10</v>
+      </c>
+      <c r="B670" t="s">
+        <v>11</v>
+      </c>
+      <c r="C670" t="s">
+        <v>0</v>
+      </c>
+      <c r="D670">
+        <v>5.96</v>
+      </c>
+      <c r="E670" t="s">
+        <v>1</v>
+      </c>
+      <c r="F670" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="671" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A671" t="s">
+        <v>10</v>
+      </c>
+      <c r="B671" t="s">
+        <v>11</v>
+      </c>
+      <c r="C671" t="s">
+        <v>0</v>
+      </c>
+      <c r="D671">
+        <v>7.19</v>
+      </c>
+      <c r="E671" t="s">
+        <v>1</v>
+      </c>
+      <c r="F671" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="672" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A672" t="s">
+        <v>10</v>
+      </c>
+      <c r="B672" t="s">
+        <v>11</v>
+      </c>
+      <c r="C672" t="s">
+        <v>0</v>
+      </c>
+      <c r="D672">
+        <v>3.07</v>
+      </c>
+      <c r="E672" t="s">
+        <v>1</v>
+      </c>
+      <c r="F672" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="673" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A673" t="s">
+        <v>10</v>
+      </c>
+      <c r="B673" t="s">
+        <v>11</v>
+      </c>
+      <c r="C673" t="s">
+        <v>0</v>
+      </c>
+      <c r="D673">
+        <v>4.8</v>
+      </c>
+      <c r="E673" t="s">
+        <v>1</v>
+      </c>
+      <c r="F673" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="674" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A674" t="s">
+        <v>10</v>
+      </c>
+      <c r="B674" t="s">
+        <v>11</v>
+      </c>
+      <c r="C674" t="s">
+        <v>0</v>
+      </c>
+      <c r="D674">
+        <v>2.98</v>
+      </c>
+      <c r="E674" t="s">
+        <v>1</v>
+      </c>
+      <c r="F674" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="675" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A675" t="s">
+        <v>10</v>
+      </c>
+      <c r="B675" t="s">
+        <v>11</v>
+      </c>
+      <c r="C675" t="s">
+        <v>0</v>
+      </c>
+      <c r="D675">
+        <v>3.04</v>
+      </c>
+      <c r="E675" t="s">
+        <v>1</v>
+      </c>
+      <c r="F675" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="676" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A676" t="s">
+        <v>2</v>
+      </c>
+      <c r="B676" t="s">
+        <v>8</v>
+      </c>
+      <c r="C676" t="s">
+        <v>0</v>
+      </c>
+      <c r="D676">
+        <v>1.6</v>
+      </c>
+      <c r="E676" t="s">
+        <v>1</v>
+      </c>
+      <c r="F676" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="677" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A677" t="s">
+        <v>2</v>
+      </c>
+      <c r="B677" t="s">
+        <v>8</v>
+      </c>
+      <c r="C677" t="s">
+        <v>0</v>
+      </c>
+      <c r="D677">
+        <v>4.59</v>
+      </c>
+      <c r="E677" t="s">
+        <v>1</v>
+      </c>
+      <c r="F677" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="678" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A678" t="s">
+        <v>2</v>
+      </c>
+      <c r="B678" t="s">
+        <v>8</v>
+      </c>
+      <c r="C678" t="s">
+        <v>0</v>
+      </c>
+      <c r="D678">
+        <v>2.71</v>
+      </c>
+      <c r="E678" t="s">
+        <v>1</v>
+      </c>
+      <c r="F678" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="679" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A679" t="s">
+        <v>2</v>
+      </c>
+      <c r="B679" t="s">
+        <v>8</v>
+      </c>
+      <c r="C679" t="s">
+        <v>0</v>
+      </c>
+      <c r="D679">
+        <v>2.91</v>
+      </c>
+      <c r="E679" t="s">
+        <v>1</v>
+      </c>
+      <c r="F679" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="680" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A680" t="s">
+        <v>2</v>
+      </c>
+      <c r="B680" t="s">
+        <v>8</v>
+      </c>
+      <c r="C680" t="s">
+        <v>0</v>
+      </c>
+      <c r="D680">
+        <v>3.09</v>
+      </c>
+      <c r="E680" t="s">
+        <v>1</v>
+      </c>
+      <c r="F680" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="681" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A681" t="s">
+        <v>2</v>
+      </c>
+      <c r="B681" t="s">
+        <v>8</v>
+      </c>
+      <c r="C681" t="s">
+        <v>0</v>
+      </c>
+      <c r="D681">
+        <v>1.78</v>
+      </c>
+      <c r="E681" t="s">
+        <v>1</v>
+      </c>
+      <c r="F681" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="682" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A682" t="s">
+        <v>2</v>
+      </c>
+      <c r="B682" t="s">
+        <v>8</v>
+      </c>
+      <c r="C682" t="s">
+        <v>0</v>
+      </c>
+      <c r="D682">
+        <v>2.84</v>
+      </c>
+      <c r="E682" t="s">
+        <v>1</v>
+      </c>
+      <c r="F682" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="683" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A683" t="s">
+        <v>2</v>
+      </c>
+      <c r="B683" t="s">
+        <v>8</v>
+      </c>
+      <c r="C683" t="s">
+        <v>0</v>
+      </c>
+      <c r="D683">
+        <v>3.68</v>
+      </c>
+      <c r="E683" t="s">
+        <v>1</v>
+      </c>
+      <c r="F683" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="684" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A684" t="s">
+        <v>2</v>
+      </c>
+      <c r="B684" t="s">
+        <v>8</v>
+      </c>
+      <c r="C684" t="s">
+        <v>0</v>
+      </c>
+      <c r="D684">
+        <v>3.56</v>
+      </c>
+      <c r="E684" t="s">
+        <v>1</v>
+      </c>
+      <c r="F684" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="685" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A685" t="s">
+        <v>2</v>
+      </c>
+      <c r="B685" t="s">
+        <v>8</v>
+      </c>
+      <c r="C685" t="s">
+        <v>0</v>
+      </c>
+      <c r="D685">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="E685" t="s">
+        <v>1</v>
+      </c>
+      <c r="F685" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="686" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A686" t="s">
+        <v>2</v>
+      </c>
+      <c r="B686" t="s">
+        <v>8</v>
+      </c>
+      <c r="C686" t="s">
+        <v>0</v>
+      </c>
+      <c r="D686">
+        <v>5.66</v>
+      </c>
+      <c r="E686" t="s">
+        <v>1</v>
+      </c>
+      <c r="F686" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="687" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A687" t="s">
+        <v>2</v>
+      </c>
+      <c r="B687" t="s">
+        <v>8</v>
+      </c>
+      <c r="C687" t="s">
+        <v>0</v>
+      </c>
+      <c r="D687">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E687" t="s">
+        <v>1</v>
+      </c>
+      <c r="F687" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="688" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A688" t="s">
+        <v>2</v>
+      </c>
+      <c r="B688" t="s">
+        <v>8</v>
+      </c>
+      <c r="C688" t="s">
+        <v>0</v>
+      </c>
+      <c r="D688">
+        <v>6.39</v>
+      </c>
+      <c r="E688" t="s">
+        <v>1</v>
+      </c>
+      <c r="F688" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="689" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A689" t="s">
+        <v>2</v>
+      </c>
+      <c r="B689" t="s">
+        <v>8</v>
+      </c>
+      <c r="C689" t="s">
+        <v>0</v>
+      </c>
+      <c r="D689">
+        <v>3.79</v>
+      </c>
+      <c r="E689" t="s">
+        <v>1</v>
+      </c>
+      <c r="F689" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="690" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A690" t="s">
+        <v>2</v>
+      </c>
+      <c r="B690" t="s">
+        <v>8</v>
+      </c>
+      <c r="C690" t="s">
+        <v>0</v>
+      </c>
+      <c r="D690">
+        <v>5.34</v>
+      </c>
+      <c r="E690" t="s">
+        <v>1</v>
+      </c>
+      <c r="F690" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="691" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A691" t="s">
+        <v>2</v>
+      </c>
+      <c r="B691" t="s">
+        <v>8</v>
+      </c>
+      <c r="C691" t="s">
+        <v>0</v>
+      </c>
+      <c r="D691">
+        <v>3.47</v>
+      </c>
+      <c r="E691" t="s">
+        <v>1</v>
+      </c>
+      <c r="F691" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="692" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A692" t="s">
+        <v>2</v>
+      </c>
+      <c r="B692" t="s">
+        <v>8</v>
+      </c>
+      <c r="C692" t="s">
+        <v>0</v>
+      </c>
+      <c r="D692">
+        <v>5.68</v>
+      </c>
+      <c r="E692" t="s">
+        <v>1</v>
+      </c>
+      <c r="F692" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="693" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>2</v>
+      </c>
+      <c r="B693" t="s">
+        <v>8</v>
+      </c>
+      <c r="C693" t="s">
+        <v>0</v>
+      </c>
+      <c r="D693">
+        <v>4.82</v>
+      </c>
+      <c r="E693" t="s">
+        <v>1</v>
+      </c>
+      <c r="F693" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="694" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A694" t="s">
+        <v>2</v>
+      </c>
+      <c r="B694" t="s">
+        <v>8</v>
+      </c>
+      <c r="C694" t="s">
+        <v>0</v>
+      </c>
+      <c r="D694">
+        <v>12.72</v>
+      </c>
+      <c r="E694" t="s">
+        <v>1</v>
+      </c>
+      <c r="F694" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="695" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A695" t="s">
+        <v>2</v>
+      </c>
+      <c r="B695" t="s">
+        <v>8</v>
+      </c>
+      <c r="C695" t="s">
+        <v>0</v>
+      </c>
+      <c r="D695">
+        <v>6.5</v>
+      </c>
+      <c r="E695" t="s">
+        <v>1</v>
+      </c>
+      <c r="F695" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="696" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A696" t="s">
+        <v>10</v>
+      </c>
+      <c r="B696" t="s">
+        <v>8</v>
+      </c>
+      <c r="C696" t="s">
+        <v>0</v>
+      </c>
+      <c r="D696">
+        <v>3.88</v>
+      </c>
+      <c r="E696" t="s">
+        <v>1</v>
+      </c>
+      <c r="F696" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="697" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A697" t="s">
+        <v>10</v>
+      </c>
+      <c r="B697" t="s">
+        <v>8</v>
+      </c>
+      <c r="C697" t="s">
+        <v>0</v>
+      </c>
+      <c r="D697">
+        <v>7.35</v>
+      </c>
+      <c r="E697" t="s">
+        <v>1</v>
+      </c>
+      <c r="F697" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="698" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A698" t="s">
+        <v>10</v>
+      </c>
+      <c r="B698" t="s">
+        <v>8</v>
+      </c>
+      <c r="C698" t="s">
+        <v>0</v>
+      </c>
+      <c r="D698">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="E698" t="s">
+        <v>1</v>
+      </c>
+      <c r="F698" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="699" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A699" t="s">
+        <v>10</v>
+      </c>
+      <c r="B699" t="s">
+        <v>8</v>
+      </c>
+      <c r="C699" t="s">
+        <v>0</v>
+      </c>
+      <c r="D699">
+        <v>6.1</v>
+      </c>
+      <c r="E699" t="s">
+        <v>1</v>
+      </c>
+      <c r="F699" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="700" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A700" t="s">
+        <v>10</v>
+      </c>
+      <c r="B700" t="s">
+        <v>8</v>
+      </c>
+      <c r="C700" t="s">
+        <v>0</v>
+      </c>
+      <c r="D700">
+        <v>4.72</v>
+      </c>
+      <c r="E700" t="s">
+        <v>1</v>
+      </c>
+      <c r="F700" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="701" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A701" t="s">
+        <v>10</v>
+      </c>
+      <c r="B701" t="s">
+        <v>8</v>
+      </c>
+      <c r="C701" t="s">
+        <v>0</v>
+      </c>
+      <c r="D701">
+        <v>6.39</v>
+      </c>
+      <c r="E701" t="s">
+        <v>1</v>
+      </c>
+      <c r="F701" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="702" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A702" t="s">
+        <v>10</v>
+      </c>
+      <c r="B702" t="s">
+        <v>8</v>
+      </c>
+      <c r="C702" t="s">
+        <v>0</v>
+      </c>
+      <c r="D702">
+        <v>5.25</v>
+      </c>
+      <c r="E702" t="s">
+        <v>1</v>
+      </c>
+      <c r="F702" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="703" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A703" t="s">
+        <v>10</v>
+      </c>
+      <c r="B703" t="s">
+        <v>8</v>
+      </c>
+      <c r="C703" t="s">
+        <v>0</v>
+      </c>
+      <c r="D703">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="E703" t="s">
+        <v>1</v>
+      </c>
+      <c r="F703" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="704" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A704" t="s">
+        <v>10</v>
+      </c>
+      <c r="B704" t="s">
+        <v>8</v>
+      </c>
+      <c r="C704" t="s">
+        <v>0</v>
+      </c>
+      <c r="D704">
+        <v>4.45</v>
+      </c>
+      <c r="E704" t="s">
+        <v>1</v>
+      </c>
+      <c r="F704" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="705" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A705" t="s">
+        <v>10</v>
+      </c>
+      <c r="B705" t="s">
+        <v>8</v>
+      </c>
+      <c r="C705" t="s">
+        <v>0</v>
+      </c>
+      <c r="D705">
+        <v>12.13</v>
+      </c>
+      <c r="E705" t="s">
+        <v>1</v>
+      </c>
+      <c r="F705" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="706" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A706" t="s">
+        <v>10</v>
+      </c>
+      <c r="B706" t="s">
+        <v>8</v>
+      </c>
+      <c r="C706" t="s">
+        <v>0</v>
+      </c>
+      <c r="D706">
+        <v>10.02</v>
+      </c>
+      <c r="E706" t="s">
+        <v>1</v>
+      </c>
+      <c r="F706" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="707" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A707" t="s">
+        <v>10</v>
+      </c>
+      <c r="B707" t="s">
+        <v>8</v>
+      </c>
+      <c r="C707" t="s">
+        <v>0</v>
+      </c>
+      <c r="D707">
+        <v>7.28</v>
+      </c>
+      <c r="E707" t="s">
+        <v>1</v>
+      </c>
+      <c r="F707" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="708" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A708" t="s">
+        <v>10</v>
+      </c>
+      <c r="B708" t="s">
+        <v>8</v>
+      </c>
+      <c r="C708" t="s">
+        <v>0</v>
+      </c>
+      <c r="D708">
+        <v>9.24</v>
+      </c>
+      <c r="E708" t="s">
+        <v>1</v>
+      </c>
+      <c r="F708" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="709" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A709" t="s">
+        <v>10</v>
+      </c>
+      <c r="B709" t="s">
+        <v>8</v>
+      </c>
+      <c r="C709" t="s">
+        <v>0</v>
+      </c>
+      <c r="D709">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E709" t="s">
+        <v>1</v>
+      </c>
+      <c r="F709" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="710" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A710" t="s">
+        <v>10</v>
+      </c>
+      <c r="B710" t="s">
+        <v>8</v>
+      </c>
+      <c r="C710" t="s">
+        <v>0</v>
+      </c>
+      <c r="D710">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E710" t="s">
+        <v>1</v>
+      </c>
+      <c r="F710" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="711" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A711" t="s">
+        <v>10</v>
+      </c>
+      <c r="B711" t="s">
+        <v>8</v>
+      </c>
+      <c r="C711" t="s">
+        <v>0</v>
+      </c>
+      <c r="D711">
+        <v>17.079999999999998</v>
+      </c>
+      <c r="E711" t="s">
+        <v>1</v>
+      </c>
+      <c r="F711" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="712" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A712" t="s">
+        <v>10</v>
+      </c>
+      <c r="B712" t="s">
+        <v>8</v>
+      </c>
+      <c r="C712" t="s">
+        <v>0</v>
+      </c>
+      <c r="D712">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E712" t="s">
+        <v>1</v>
+      </c>
+      <c r="F712" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="713" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A713" t="s">
+        <v>10</v>
+      </c>
+      <c r="B713" t="s">
+        <v>8</v>
+      </c>
+      <c r="C713" t="s">
+        <v>0</v>
+      </c>
+      <c r="D713">
+        <v>1.44</v>
+      </c>
+      <c r="E713" t="s">
+        <v>1</v>
+      </c>
+      <c r="F713" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="714" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A714" t="s">
+        <v>10</v>
+      </c>
+      <c r="B714" t="s">
+        <v>8</v>
+      </c>
+      <c r="C714" t="s">
+        <v>0</v>
+      </c>
+      <c r="D714">
+        <v>2.4</v>
+      </c>
+      <c r="E714" t="s">
+        <v>1</v>
+      </c>
+      <c r="F714" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="715" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A715" t="s">
+        <v>10</v>
+      </c>
+      <c r="B715" t="s">
+        <v>8</v>
+      </c>
+      <c r="C715" t="s">
+        <v>0</v>
+      </c>
+      <c r="D715">
+        <v>3.6</v>
+      </c>
+      <c r="E715" t="s">
+        <v>1</v>
+      </c>
+      <c r="F715" s="1">
+        <v>44838</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TB suppresion assay 10/13
</commit_message>
<xml_diff>
--- a/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
+++ b/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiabrown/Documents/git/cest-2.1-Project/Tia_Jub39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B1FDD6-AC00-E54C-88F0-4C75B2169D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436EAADC-8BAE-C44E-AF84-A8BC61A14185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15600" xr2:uid="{DD7AC6D9-FEFD-0E41-A755-99DADF736280}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2862" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3810" uniqueCount="14">
   <si>
     <t>100pct</t>
   </si>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A9CC03-DE84-E245-89A8-02F35FB81FD2}">
-  <dimension ref="A1:F715"/>
+  <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A681" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G704" sqref="G704"/>
+    <sheetView tabSelected="1" topLeftCell="A929" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H936" sqref="H936"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14756,6 +14756,4746 @@
         <v>44838</v>
       </c>
     </row>
+    <row r="716" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A716" t="s">
+        <v>10</v>
+      </c>
+      <c r="B716" t="s">
+        <v>8</v>
+      </c>
+      <c r="C716" t="s">
+        <v>0</v>
+      </c>
+      <c r="D716">
+        <v>2.39</v>
+      </c>
+      <c r="E716" t="s">
+        <v>13</v>
+      </c>
+      <c r="F716" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="717" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A717" t="s">
+        <v>10</v>
+      </c>
+      <c r="B717" t="s">
+        <v>8</v>
+      </c>
+      <c r="C717" t="s">
+        <v>0</v>
+      </c>
+      <c r="D717">
+        <v>3.44</v>
+      </c>
+      <c r="E717" t="s">
+        <v>13</v>
+      </c>
+      <c r="F717" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="718" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A718" t="s">
+        <v>10</v>
+      </c>
+      <c r="B718" t="s">
+        <v>8</v>
+      </c>
+      <c r="C718" t="s">
+        <v>0</v>
+      </c>
+      <c r="D718">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E718" t="s">
+        <v>13</v>
+      </c>
+      <c r="F718" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="719" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A719" t="s">
+        <v>10</v>
+      </c>
+      <c r="B719" t="s">
+        <v>8</v>
+      </c>
+      <c r="C719" t="s">
+        <v>0</v>
+      </c>
+      <c r="D719">
+        <v>3.23</v>
+      </c>
+      <c r="E719" t="s">
+        <v>13</v>
+      </c>
+      <c r="F719" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="720" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A720" t="s">
+        <v>10</v>
+      </c>
+      <c r="B720" t="s">
+        <v>8</v>
+      </c>
+      <c r="C720" t="s">
+        <v>0</v>
+      </c>
+      <c r="D720">
+        <v>2.38</v>
+      </c>
+      <c r="E720" t="s">
+        <v>13</v>
+      </c>
+      <c r="F720" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="721" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A721" t="s">
+        <v>10</v>
+      </c>
+      <c r="B721" t="s">
+        <v>8</v>
+      </c>
+      <c r="C721" t="s">
+        <v>0</v>
+      </c>
+      <c r="D721">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E721" t="s">
+        <v>13</v>
+      </c>
+      <c r="F721" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="722" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A722" t="s">
+        <v>10</v>
+      </c>
+      <c r="B722" t="s">
+        <v>8</v>
+      </c>
+      <c r="C722" t="s">
+        <v>0</v>
+      </c>
+      <c r="D722">
+        <v>2.71</v>
+      </c>
+      <c r="E722" t="s">
+        <v>13</v>
+      </c>
+      <c r="F722" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="723" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A723" t="s">
+        <v>10</v>
+      </c>
+      <c r="B723" t="s">
+        <v>8</v>
+      </c>
+      <c r="C723" t="s">
+        <v>0</v>
+      </c>
+      <c r="D723">
+        <v>13.54</v>
+      </c>
+      <c r="E723" t="s">
+        <v>13</v>
+      </c>
+      <c r="F723" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="724" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A724" t="s">
+        <v>10</v>
+      </c>
+      <c r="B724" t="s">
+        <v>8</v>
+      </c>
+      <c r="C724" t="s">
+        <v>0</v>
+      </c>
+      <c r="D724">
+        <v>2.68</v>
+      </c>
+      <c r="E724" t="s">
+        <v>13</v>
+      </c>
+      <c r="F724" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="725" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A725" t="s">
+        <v>10</v>
+      </c>
+      <c r="B725" t="s">
+        <v>8</v>
+      </c>
+      <c r="C725" t="s">
+        <v>0</v>
+      </c>
+      <c r="D725">
+        <v>1.68</v>
+      </c>
+      <c r="E725" t="s">
+        <v>13</v>
+      </c>
+      <c r="F725" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="726" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A726" t="s">
+        <v>10</v>
+      </c>
+      <c r="B726" t="s">
+        <v>8</v>
+      </c>
+      <c r="C726" t="s">
+        <v>0</v>
+      </c>
+      <c r="D726">
+        <v>2.93</v>
+      </c>
+      <c r="E726" t="s">
+        <v>13</v>
+      </c>
+      <c r="F726" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="727" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A727" t="s">
+        <v>10</v>
+      </c>
+      <c r="B727" t="s">
+        <v>8</v>
+      </c>
+      <c r="C727" t="s">
+        <v>0</v>
+      </c>
+      <c r="D727">
+        <v>3.13</v>
+      </c>
+      <c r="E727" t="s">
+        <v>13</v>
+      </c>
+      <c r="F727" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="728" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A728" t="s">
+        <v>10</v>
+      </c>
+      <c r="B728" t="s">
+        <v>8</v>
+      </c>
+      <c r="C728" t="s">
+        <v>0</v>
+      </c>
+      <c r="D728">
+        <v>2.14</v>
+      </c>
+      <c r="E728" t="s">
+        <v>13</v>
+      </c>
+      <c r="F728" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="729" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A729" t="s">
+        <v>10</v>
+      </c>
+      <c r="B729" t="s">
+        <v>8</v>
+      </c>
+      <c r="C729" t="s">
+        <v>0</v>
+      </c>
+      <c r="D729">
+        <v>5.99</v>
+      </c>
+      <c r="E729" t="s">
+        <v>13</v>
+      </c>
+      <c r="F729" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="730" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A730" t="s">
+        <v>10</v>
+      </c>
+      <c r="B730" t="s">
+        <v>8</v>
+      </c>
+      <c r="C730" t="s">
+        <v>0</v>
+      </c>
+      <c r="D730">
+        <v>10.41</v>
+      </c>
+      <c r="E730" t="s">
+        <v>13</v>
+      </c>
+      <c r="F730" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="731" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A731" t="s">
+        <v>10</v>
+      </c>
+      <c r="B731" t="s">
+        <v>8</v>
+      </c>
+      <c r="C731" t="s">
+        <v>0</v>
+      </c>
+      <c r="D731">
+        <v>4.13</v>
+      </c>
+      <c r="E731" t="s">
+        <v>13</v>
+      </c>
+      <c r="F731" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="732" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A732" t="s">
+        <v>2</v>
+      </c>
+      <c r="B732" t="s">
+        <v>8</v>
+      </c>
+      <c r="C732" t="s">
+        <v>0</v>
+      </c>
+      <c r="D732">
+        <v>3.31</v>
+      </c>
+      <c r="E732" t="s">
+        <v>13</v>
+      </c>
+      <c r="F732" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="733" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A733" t="s">
+        <v>2</v>
+      </c>
+      <c r="B733" t="s">
+        <v>8</v>
+      </c>
+      <c r="C733" t="s">
+        <v>0</v>
+      </c>
+      <c r="D733">
+        <v>2.56</v>
+      </c>
+      <c r="E733" t="s">
+        <v>13</v>
+      </c>
+      <c r="F733" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="734" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A734" t="s">
+        <v>2</v>
+      </c>
+      <c r="B734" t="s">
+        <v>8</v>
+      </c>
+      <c r="C734" t="s">
+        <v>0</v>
+      </c>
+      <c r="D734">
+        <v>3.61</v>
+      </c>
+      <c r="E734" t="s">
+        <v>13</v>
+      </c>
+      <c r="F734" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="735" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A735" t="s">
+        <v>2</v>
+      </c>
+      <c r="B735" t="s">
+        <v>8</v>
+      </c>
+      <c r="C735" t="s">
+        <v>0</v>
+      </c>
+      <c r="D735">
+        <v>3.11</v>
+      </c>
+      <c r="E735" t="s">
+        <v>13</v>
+      </c>
+      <c r="F735" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="736" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A736" t="s">
+        <v>2</v>
+      </c>
+      <c r="B736" t="s">
+        <v>8</v>
+      </c>
+      <c r="C736" t="s">
+        <v>0</v>
+      </c>
+      <c r="D736">
+        <v>6.64</v>
+      </c>
+      <c r="E736" t="s">
+        <v>13</v>
+      </c>
+      <c r="F736" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="737" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A737" t="s">
+        <v>2</v>
+      </c>
+      <c r="B737" t="s">
+        <v>8</v>
+      </c>
+      <c r="C737" t="s">
+        <v>0</v>
+      </c>
+      <c r="D737">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="E737" t="s">
+        <v>13</v>
+      </c>
+      <c r="F737" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="738" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A738" t="s">
+        <v>2</v>
+      </c>
+      <c r="B738" t="s">
+        <v>8</v>
+      </c>
+      <c r="C738" t="s">
+        <v>0</v>
+      </c>
+      <c r="D738">
+        <v>9.94</v>
+      </c>
+      <c r="E738" t="s">
+        <v>13</v>
+      </c>
+      <c r="F738" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="739" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A739" t="s">
+        <v>2</v>
+      </c>
+      <c r="B739" t="s">
+        <v>8</v>
+      </c>
+      <c r="C739" t="s">
+        <v>0</v>
+      </c>
+      <c r="D739">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E739" t="s">
+        <v>13</v>
+      </c>
+      <c r="F739" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="740" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A740" t="s">
+        <v>2</v>
+      </c>
+      <c r="B740" t="s">
+        <v>8</v>
+      </c>
+      <c r="C740" t="s">
+        <v>0</v>
+      </c>
+      <c r="D740">
+        <v>2.84</v>
+      </c>
+      <c r="E740" t="s">
+        <v>13</v>
+      </c>
+      <c r="F740" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="741" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A741" t="s">
+        <v>2</v>
+      </c>
+      <c r="B741" t="s">
+        <v>8</v>
+      </c>
+      <c r="C741" t="s">
+        <v>0</v>
+      </c>
+      <c r="D741">
+        <v>11.66</v>
+      </c>
+      <c r="E741" t="s">
+        <v>13</v>
+      </c>
+      <c r="F741" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="742" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A742" t="s">
+        <v>2</v>
+      </c>
+      <c r="B742" t="s">
+        <v>8</v>
+      </c>
+      <c r="C742" t="s">
+        <v>0</v>
+      </c>
+      <c r="D742">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="E742" t="s">
+        <v>13</v>
+      </c>
+      <c r="F742" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="743" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A743" t="s">
+        <v>10</v>
+      </c>
+      <c r="B743" t="s">
+        <v>11</v>
+      </c>
+      <c r="C743" t="s">
+        <v>0</v>
+      </c>
+      <c r="D743">
+        <v>2.58</v>
+      </c>
+      <c r="E743" t="s">
+        <v>13</v>
+      </c>
+      <c r="F743" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="744" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A744" t="s">
+        <v>10</v>
+      </c>
+      <c r="B744" t="s">
+        <v>11</v>
+      </c>
+      <c r="C744" t="s">
+        <v>0</v>
+      </c>
+      <c r="D744">
+        <v>3.44</v>
+      </c>
+      <c r="E744" t="s">
+        <v>13</v>
+      </c>
+      <c r="F744" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="745" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A745" t="s">
+        <v>10</v>
+      </c>
+      <c r="B745" t="s">
+        <v>11</v>
+      </c>
+      <c r="C745" t="s">
+        <v>0</v>
+      </c>
+      <c r="D745">
+        <v>3.44</v>
+      </c>
+      <c r="E745" t="s">
+        <v>13</v>
+      </c>
+      <c r="F745" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="746" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A746" t="s">
+        <v>10</v>
+      </c>
+      <c r="B746" t="s">
+        <v>11</v>
+      </c>
+      <c r="C746" t="s">
+        <v>0</v>
+      </c>
+      <c r="D746">
+        <v>6.44</v>
+      </c>
+      <c r="E746" t="s">
+        <v>13</v>
+      </c>
+      <c r="F746" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="747" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A747" t="s">
+        <v>10</v>
+      </c>
+      <c r="B747" t="s">
+        <v>11</v>
+      </c>
+      <c r="C747" t="s">
+        <v>0</v>
+      </c>
+      <c r="D747">
+        <v>3.21</v>
+      </c>
+      <c r="E747" t="s">
+        <v>13</v>
+      </c>
+      <c r="F747" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="748" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A748" t="s">
+        <v>10</v>
+      </c>
+      <c r="B748" t="s">
+        <v>11</v>
+      </c>
+      <c r="C748" t="s">
+        <v>0</v>
+      </c>
+      <c r="D748">
+        <v>2.41</v>
+      </c>
+      <c r="E748" t="s">
+        <v>13</v>
+      </c>
+      <c r="F748" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="749" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A749" t="s">
+        <v>10</v>
+      </c>
+      <c r="B749" t="s">
+        <v>11</v>
+      </c>
+      <c r="C749" t="s">
+        <v>0</v>
+      </c>
+      <c r="D749">
+        <v>5.51</v>
+      </c>
+      <c r="E749" t="s">
+        <v>13</v>
+      </c>
+      <c r="F749" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="750" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A750" t="s">
+        <v>10</v>
+      </c>
+      <c r="B750" t="s">
+        <v>11</v>
+      </c>
+      <c r="C750" t="s">
+        <v>0</v>
+      </c>
+      <c r="D750">
+        <v>3.28</v>
+      </c>
+      <c r="E750" t="s">
+        <v>13</v>
+      </c>
+      <c r="F750" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="751" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A751" t="s">
+        <v>10</v>
+      </c>
+      <c r="B751" t="s">
+        <v>11</v>
+      </c>
+      <c r="C751" t="s">
+        <v>0</v>
+      </c>
+      <c r="D751">
+        <v>2.96</v>
+      </c>
+      <c r="E751" t="s">
+        <v>13</v>
+      </c>
+      <c r="F751" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="752" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A752" t="s">
+        <v>10</v>
+      </c>
+      <c r="B752" t="s">
+        <v>11</v>
+      </c>
+      <c r="C752" t="s">
+        <v>0</v>
+      </c>
+      <c r="D752">
+        <v>2.06</v>
+      </c>
+      <c r="E752" t="s">
+        <v>13</v>
+      </c>
+      <c r="F752" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="753" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A753" t="s">
+        <v>10</v>
+      </c>
+      <c r="B753" t="s">
+        <v>11</v>
+      </c>
+      <c r="C753" t="s">
+        <v>0</v>
+      </c>
+      <c r="D753">
+        <v>2.69</v>
+      </c>
+      <c r="E753" t="s">
+        <v>13</v>
+      </c>
+      <c r="F753" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="754" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A754" t="s">
+        <v>10</v>
+      </c>
+      <c r="B754" t="s">
+        <v>11</v>
+      </c>
+      <c r="C754" t="s">
+        <v>0</v>
+      </c>
+      <c r="D754">
+        <v>4.83</v>
+      </c>
+      <c r="E754" t="s">
+        <v>13</v>
+      </c>
+      <c r="F754" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="755" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A755" t="s">
+        <v>10</v>
+      </c>
+      <c r="B755" t="s">
+        <v>11</v>
+      </c>
+      <c r="C755" t="s">
+        <v>0</v>
+      </c>
+      <c r="D755">
+        <v>3.83</v>
+      </c>
+      <c r="E755" t="s">
+        <v>13</v>
+      </c>
+      <c r="F755" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="756" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A756" t="s">
+        <v>10</v>
+      </c>
+      <c r="B756" t="s">
+        <v>11</v>
+      </c>
+      <c r="C756" t="s">
+        <v>0</v>
+      </c>
+      <c r="D756">
+        <v>1.48</v>
+      </c>
+      <c r="E756" t="s">
+        <v>13</v>
+      </c>
+      <c r="F756" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="757" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A757" t="s">
+        <v>10</v>
+      </c>
+      <c r="B757" t="s">
+        <v>11</v>
+      </c>
+      <c r="C757" t="s">
+        <v>0</v>
+      </c>
+      <c r="D757">
+        <v>1.76</v>
+      </c>
+      <c r="E757" t="s">
+        <v>13</v>
+      </c>
+      <c r="F757" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="758" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A758" t="s">
+        <v>10</v>
+      </c>
+      <c r="B758" t="s">
+        <v>11</v>
+      </c>
+      <c r="C758" t="s">
+        <v>0</v>
+      </c>
+      <c r="D758">
+        <v>3.11</v>
+      </c>
+      <c r="E758" t="s">
+        <v>13</v>
+      </c>
+      <c r="F758" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="759" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A759" t="s">
+        <v>10</v>
+      </c>
+      <c r="B759" t="s">
+        <v>11</v>
+      </c>
+      <c r="C759" t="s">
+        <v>0</v>
+      </c>
+      <c r="D759">
+        <v>10.11</v>
+      </c>
+      <c r="E759" t="s">
+        <v>13</v>
+      </c>
+      <c r="F759" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="760" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A760" t="s">
+        <v>2</v>
+      </c>
+      <c r="B760" t="s">
+        <v>11</v>
+      </c>
+      <c r="C760" t="s">
+        <v>0</v>
+      </c>
+      <c r="D760">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E760" t="s">
+        <v>13</v>
+      </c>
+      <c r="F760" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="761" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A761" t="s">
+        <v>2</v>
+      </c>
+      <c r="B761" t="s">
+        <v>11</v>
+      </c>
+      <c r="C761" t="s">
+        <v>0</v>
+      </c>
+      <c r="D761">
+        <v>3.16</v>
+      </c>
+      <c r="E761" t="s">
+        <v>13</v>
+      </c>
+      <c r="F761" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="762" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A762" t="s">
+        <v>2</v>
+      </c>
+      <c r="B762" t="s">
+        <v>11</v>
+      </c>
+      <c r="C762" t="s">
+        <v>0</v>
+      </c>
+      <c r="D762">
+        <v>3.06</v>
+      </c>
+      <c r="E762" t="s">
+        <v>13</v>
+      </c>
+      <c r="F762" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="763" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A763" t="s">
+        <v>2</v>
+      </c>
+      <c r="B763" t="s">
+        <v>11</v>
+      </c>
+      <c r="C763" t="s">
+        <v>0</v>
+      </c>
+      <c r="D763">
+        <v>2.29</v>
+      </c>
+      <c r="E763" t="s">
+        <v>13</v>
+      </c>
+      <c r="F763" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="764" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A764" t="s">
+        <v>2</v>
+      </c>
+      <c r="B764" t="s">
+        <v>11</v>
+      </c>
+      <c r="C764" t="s">
+        <v>0</v>
+      </c>
+      <c r="D764">
+        <v>6.94</v>
+      </c>
+      <c r="E764" t="s">
+        <v>13</v>
+      </c>
+      <c r="F764" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="765" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A765" t="s">
+        <v>2</v>
+      </c>
+      <c r="B765" t="s">
+        <v>11</v>
+      </c>
+      <c r="C765" t="s">
+        <v>0</v>
+      </c>
+      <c r="D765">
+        <v>2.39</v>
+      </c>
+      <c r="E765" t="s">
+        <v>13</v>
+      </c>
+      <c r="F765" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="766" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A766" t="s">
+        <v>2</v>
+      </c>
+      <c r="B766" t="s">
+        <v>11</v>
+      </c>
+      <c r="C766" t="s">
+        <v>0</v>
+      </c>
+      <c r="D766">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="E766" t="s">
+        <v>13</v>
+      </c>
+      <c r="F766" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="767" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A767" t="s">
+        <v>2</v>
+      </c>
+      <c r="B767" t="s">
+        <v>11</v>
+      </c>
+      <c r="C767" t="s">
+        <v>0</v>
+      </c>
+      <c r="D767">
+        <v>16.88</v>
+      </c>
+      <c r="E767" t="s">
+        <v>13</v>
+      </c>
+      <c r="F767" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="768" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A768" t="s">
+        <v>2</v>
+      </c>
+      <c r="B768" t="s">
+        <v>11</v>
+      </c>
+      <c r="C768" t="s">
+        <v>0</v>
+      </c>
+      <c r="D768">
+        <v>2.54</v>
+      </c>
+      <c r="E768" t="s">
+        <v>13</v>
+      </c>
+      <c r="F768" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="769" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A769" t="s">
+        <v>2</v>
+      </c>
+      <c r="B769" t="s">
+        <v>11</v>
+      </c>
+      <c r="C769" t="s">
+        <v>0</v>
+      </c>
+      <c r="D769">
+        <v>3.94</v>
+      </c>
+      <c r="E769" t="s">
+        <v>13</v>
+      </c>
+      <c r="F769" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="770" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A770" t="s">
+        <v>2</v>
+      </c>
+      <c r="B770" t="s">
+        <v>11</v>
+      </c>
+      <c r="C770" t="s">
+        <v>0</v>
+      </c>
+      <c r="D770">
+        <v>2.84</v>
+      </c>
+      <c r="E770" t="s">
+        <v>13</v>
+      </c>
+      <c r="F770" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="771" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A771" t="s">
+        <v>2</v>
+      </c>
+      <c r="B771" t="s">
+        <v>11</v>
+      </c>
+      <c r="C771" t="s">
+        <v>0</v>
+      </c>
+      <c r="D771">
+        <v>3.59</v>
+      </c>
+      <c r="E771" t="s">
+        <v>13</v>
+      </c>
+      <c r="F771" s="1">
+        <v>44810</v>
+      </c>
+    </row>
+    <row r="772" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A772" t="s">
+        <v>10</v>
+      </c>
+      <c r="B772" t="s">
+        <v>8</v>
+      </c>
+      <c r="C772" t="s">
+        <v>0</v>
+      </c>
+      <c r="D772">
+        <v>3.5</v>
+      </c>
+      <c r="E772" t="s">
+        <v>13</v>
+      </c>
+      <c r="F772" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="773" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A773" t="s">
+        <v>10</v>
+      </c>
+      <c r="B773" t="s">
+        <v>8</v>
+      </c>
+      <c r="C773" t="s">
+        <v>0</v>
+      </c>
+      <c r="D773">
+        <v>2.1</v>
+      </c>
+      <c r="E773" t="s">
+        <v>13</v>
+      </c>
+      <c r="F773" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="774" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A774" t="s">
+        <v>10</v>
+      </c>
+      <c r="B774" t="s">
+        <v>8</v>
+      </c>
+      <c r="C774" t="s">
+        <v>0</v>
+      </c>
+      <c r="D774">
+        <v>2.4</v>
+      </c>
+      <c r="E774" t="s">
+        <v>13</v>
+      </c>
+      <c r="F774" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="775" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A775" t="s">
+        <v>10</v>
+      </c>
+      <c r="B775" t="s">
+        <v>8</v>
+      </c>
+      <c r="C775" t="s">
+        <v>0</v>
+      </c>
+      <c r="D775">
+        <v>9.4</v>
+      </c>
+      <c r="E775" t="s">
+        <v>13</v>
+      </c>
+      <c r="F775" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="776" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A776" t="s">
+        <v>10</v>
+      </c>
+      <c r="B776" t="s">
+        <v>8</v>
+      </c>
+      <c r="C776" t="s">
+        <v>0</v>
+      </c>
+      <c r="D776">
+        <v>3</v>
+      </c>
+      <c r="E776" t="s">
+        <v>13</v>
+      </c>
+      <c r="F776" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="777" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A777" t="s">
+        <v>10</v>
+      </c>
+      <c r="B777" t="s">
+        <v>8</v>
+      </c>
+      <c r="C777" t="s">
+        <v>0</v>
+      </c>
+      <c r="D777">
+        <v>2.8</v>
+      </c>
+      <c r="E777" t="s">
+        <v>13</v>
+      </c>
+      <c r="F777" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="778" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A778" t="s">
+        <v>10</v>
+      </c>
+      <c r="B778" t="s">
+        <v>8</v>
+      </c>
+      <c r="C778" t="s">
+        <v>0</v>
+      </c>
+      <c r="D778">
+        <v>2.7</v>
+      </c>
+      <c r="E778" t="s">
+        <v>13</v>
+      </c>
+      <c r="F778" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="779" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A779" t="s">
+        <v>10</v>
+      </c>
+      <c r="B779" t="s">
+        <v>8</v>
+      </c>
+      <c r="C779" t="s">
+        <v>0</v>
+      </c>
+      <c r="D779">
+        <v>4.7</v>
+      </c>
+      <c r="E779" t="s">
+        <v>13</v>
+      </c>
+      <c r="F779" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="780" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A780" t="s">
+        <v>10</v>
+      </c>
+      <c r="B780" t="s">
+        <v>8</v>
+      </c>
+      <c r="C780" t="s">
+        <v>0</v>
+      </c>
+      <c r="D780">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E780" t="s">
+        <v>13</v>
+      </c>
+      <c r="F780" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="781" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A781" t="s">
+        <v>10</v>
+      </c>
+      <c r="B781" t="s">
+        <v>8</v>
+      </c>
+      <c r="C781" t="s">
+        <v>0</v>
+      </c>
+      <c r="D781">
+        <v>6.9</v>
+      </c>
+      <c r="E781" t="s">
+        <v>13</v>
+      </c>
+      <c r="F781" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="782" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A782" t="s">
+        <v>10</v>
+      </c>
+      <c r="B782" t="s">
+        <v>8</v>
+      </c>
+      <c r="C782" t="s">
+        <v>0</v>
+      </c>
+      <c r="D782">
+        <v>1.9</v>
+      </c>
+      <c r="E782" t="s">
+        <v>13</v>
+      </c>
+      <c r="F782" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="783" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A783" t="s">
+        <v>10</v>
+      </c>
+      <c r="B783" t="s">
+        <v>8</v>
+      </c>
+      <c r="C783" t="s">
+        <v>0</v>
+      </c>
+      <c r="D783">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E783" t="s">
+        <v>13</v>
+      </c>
+      <c r="F783" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="784" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A784" t="s">
+        <v>10</v>
+      </c>
+      <c r="B784" t="s">
+        <v>8</v>
+      </c>
+      <c r="C784" t="s">
+        <v>0</v>
+      </c>
+      <c r="D784">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E784" t="s">
+        <v>13</v>
+      </c>
+      <c r="F784" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="785" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A785" t="s">
+        <v>10</v>
+      </c>
+      <c r="B785" t="s">
+        <v>8</v>
+      </c>
+      <c r="C785" t="s">
+        <v>0</v>
+      </c>
+      <c r="D785">
+        <v>4</v>
+      </c>
+      <c r="E785" t="s">
+        <v>13</v>
+      </c>
+      <c r="F785" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="786" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A786" t="s">
+        <v>10</v>
+      </c>
+      <c r="B786" t="s">
+        <v>8</v>
+      </c>
+      <c r="C786" t="s">
+        <v>0</v>
+      </c>
+      <c r="D786">
+        <v>2.1</v>
+      </c>
+      <c r="E786" t="s">
+        <v>13</v>
+      </c>
+      <c r="F786" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="787" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A787" t="s">
+        <v>2</v>
+      </c>
+      <c r="B787" t="s">
+        <v>8</v>
+      </c>
+      <c r="C787" t="s">
+        <v>0</v>
+      </c>
+      <c r="D787">
+        <v>5.7</v>
+      </c>
+      <c r="E787" t="s">
+        <v>13</v>
+      </c>
+      <c r="F787" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="788" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A788" t="s">
+        <v>2</v>
+      </c>
+      <c r="B788" t="s">
+        <v>8</v>
+      </c>
+      <c r="C788" t="s">
+        <v>0</v>
+      </c>
+      <c r="D788">
+        <v>6.1</v>
+      </c>
+      <c r="E788" t="s">
+        <v>13</v>
+      </c>
+      <c r="F788" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="789" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A789" t="s">
+        <v>2</v>
+      </c>
+      <c r="B789" t="s">
+        <v>8</v>
+      </c>
+      <c r="C789" t="s">
+        <v>0</v>
+      </c>
+      <c r="D789">
+        <v>3.2</v>
+      </c>
+      <c r="E789" t="s">
+        <v>13</v>
+      </c>
+      <c r="F789" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="790" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A790" t="s">
+        <v>2</v>
+      </c>
+      <c r="B790" t="s">
+        <v>8</v>
+      </c>
+      <c r="C790" t="s">
+        <v>0</v>
+      </c>
+      <c r="D790">
+        <v>1.9</v>
+      </c>
+      <c r="E790" t="s">
+        <v>13</v>
+      </c>
+      <c r="F790" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="791" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A791" t="s">
+        <v>2</v>
+      </c>
+      <c r="B791" t="s">
+        <v>8</v>
+      </c>
+      <c r="C791" t="s">
+        <v>0</v>
+      </c>
+      <c r="D791">
+        <v>3.5</v>
+      </c>
+      <c r="E791" t="s">
+        <v>13</v>
+      </c>
+      <c r="F791" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="792" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A792" t="s">
+        <v>2</v>
+      </c>
+      <c r="B792" t="s">
+        <v>8</v>
+      </c>
+      <c r="C792" t="s">
+        <v>0</v>
+      </c>
+      <c r="D792">
+        <v>17.3</v>
+      </c>
+      <c r="E792" t="s">
+        <v>13</v>
+      </c>
+      <c r="F792" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="793" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A793" t="s">
+        <v>2</v>
+      </c>
+      <c r="B793" t="s">
+        <v>8</v>
+      </c>
+      <c r="C793" t="s">
+        <v>0</v>
+      </c>
+      <c r="D793">
+        <v>14</v>
+      </c>
+      <c r="E793" t="s">
+        <v>13</v>
+      </c>
+      <c r="F793" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="794" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A794" t="s">
+        <v>2</v>
+      </c>
+      <c r="B794" t="s">
+        <v>8</v>
+      </c>
+      <c r="C794" t="s">
+        <v>0</v>
+      </c>
+      <c r="D794">
+        <v>19.7</v>
+      </c>
+      <c r="E794" t="s">
+        <v>13</v>
+      </c>
+      <c r="F794" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="795" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A795" t="s">
+        <v>2</v>
+      </c>
+      <c r="B795" t="s">
+        <v>8</v>
+      </c>
+      <c r="C795" t="s">
+        <v>0</v>
+      </c>
+      <c r="D795">
+        <v>2.7</v>
+      </c>
+      <c r="E795" t="s">
+        <v>13</v>
+      </c>
+      <c r="F795" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="796" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A796" t="s">
+        <v>2</v>
+      </c>
+      <c r="B796" t="s">
+        <v>8</v>
+      </c>
+      <c r="C796" t="s">
+        <v>0</v>
+      </c>
+      <c r="D796">
+        <v>2.4</v>
+      </c>
+      <c r="E796" t="s">
+        <v>13</v>
+      </c>
+      <c r="F796" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="797" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A797" t="s">
+        <v>2</v>
+      </c>
+      <c r="B797" t="s">
+        <v>8</v>
+      </c>
+      <c r="C797" t="s">
+        <v>0</v>
+      </c>
+      <c r="D797">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E797" t="s">
+        <v>13</v>
+      </c>
+      <c r="F797" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="798" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A798" t="s">
+        <v>2</v>
+      </c>
+      <c r="B798" t="s">
+        <v>8</v>
+      </c>
+      <c r="C798" t="s">
+        <v>0</v>
+      </c>
+      <c r="D798">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E798" t="s">
+        <v>13</v>
+      </c>
+      <c r="F798" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="799" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A799" t="s">
+        <v>2</v>
+      </c>
+      <c r="B799" t="s">
+        <v>8</v>
+      </c>
+      <c r="C799" t="s">
+        <v>0</v>
+      </c>
+      <c r="D799">
+        <v>11</v>
+      </c>
+      <c r="E799" t="s">
+        <v>13</v>
+      </c>
+      <c r="F799" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="800" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A800" t="s">
+        <v>10</v>
+      </c>
+      <c r="B800" t="s">
+        <v>11</v>
+      </c>
+      <c r="C800" t="s">
+        <v>0</v>
+      </c>
+      <c r="D800">
+        <v>8</v>
+      </c>
+      <c r="E800" t="s">
+        <v>13</v>
+      </c>
+      <c r="F800" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="801" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A801" t="s">
+        <v>10</v>
+      </c>
+      <c r="B801" t="s">
+        <v>11</v>
+      </c>
+      <c r="C801" t="s">
+        <v>0</v>
+      </c>
+      <c r="D801">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E801" t="s">
+        <v>13</v>
+      </c>
+      <c r="F801" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="802" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A802" t="s">
+        <v>10</v>
+      </c>
+      <c r="B802" t="s">
+        <v>11</v>
+      </c>
+      <c r="C802" t="s">
+        <v>0</v>
+      </c>
+      <c r="D802">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E802" t="s">
+        <v>13</v>
+      </c>
+      <c r="F802" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="803" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A803" t="s">
+        <v>10</v>
+      </c>
+      <c r="B803" t="s">
+        <v>11</v>
+      </c>
+      <c r="C803" t="s">
+        <v>0</v>
+      </c>
+      <c r="D803">
+        <v>2.8</v>
+      </c>
+      <c r="E803" t="s">
+        <v>13</v>
+      </c>
+      <c r="F803" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="804" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A804" t="s">
+        <v>10</v>
+      </c>
+      <c r="B804" t="s">
+        <v>11</v>
+      </c>
+      <c r="C804" t="s">
+        <v>0</v>
+      </c>
+      <c r="D804">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E804" t="s">
+        <v>13</v>
+      </c>
+      <c r="F804" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="805" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A805" t="s">
+        <v>10</v>
+      </c>
+      <c r="B805" t="s">
+        <v>11</v>
+      </c>
+      <c r="C805" t="s">
+        <v>0</v>
+      </c>
+      <c r="D805">
+        <v>3.2</v>
+      </c>
+      <c r="E805" t="s">
+        <v>13</v>
+      </c>
+      <c r="F805" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="806" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A806" t="s">
+        <v>10</v>
+      </c>
+      <c r="B806" t="s">
+        <v>11</v>
+      </c>
+      <c r="C806" t="s">
+        <v>0</v>
+      </c>
+      <c r="D806">
+        <v>6.2</v>
+      </c>
+      <c r="E806" t="s">
+        <v>13</v>
+      </c>
+      <c r="F806" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="807" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A807" t="s">
+        <v>10</v>
+      </c>
+      <c r="B807" t="s">
+        <v>11</v>
+      </c>
+      <c r="C807" t="s">
+        <v>0</v>
+      </c>
+      <c r="D807">
+        <v>13.5</v>
+      </c>
+      <c r="E807" t="s">
+        <v>13</v>
+      </c>
+      <c r="F807" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="808" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A808" t="s">
+        <v>10</v>
+      </c>
+      <c r="B808" t="s">
+        <v>11</v>
+      </c>
+      <c r="C808" t="s">
+        <v>0</v>
+      </c>
+      <c r="D808">
+        <v>14.4</v>
+      </c>
+      <c r="E808" t="s">
+        <v>13</v>
+      </c>
+      <c r="F808" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="809" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>10</v>
+      </c>
+      <c r="B809" t="s">
+        <v>11</v>
+      </c>
+      <c r="C809" t="s">
+        <v>0</v>
+      </c>
+      <c r="D809">
+        <v>6.3</v>
+      </c>
+      <c r="E809" t="s">
+        <v>13</v>
+      </c>
+      <c r="F809" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="810" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>10</v>
+      </c>
+      <c r="B810" t="s">
+        <v>11</v>
+      </c>
+      <c r="C810" t="s">
+        <v>0</v>
+      </c>
+      <c r="D810">
+        <v>4.3</v>
+      </c>
+      <c r="E810" t="s">
+        <v>13</v>
+      </c>
+      <c r="F810" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="811" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A811" t="s">
+        <v>10</v>
+      </c>
+      <c r="B811" t="s">
+        <v>11</v>
+      </c>
+      <c r="C811" t="s">
+        <v>0</v>
+      </c>
+      <c r="D811">
+        <v>6.8</v>
+      </c>
+      <c r="E811" t="s">
+        <v>13</v>
+      </c>
+      <c r="F811" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="812" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A812" t="s">
+        <v>10</v>
+      </c>
+      <c r="B812" t="s">
+        <v>11</v>
+      </c>
+      <c r="C812" t="s">
+        <v>0</v>
+      </c>
+      <c r="D812">
+        <v>3.9</v>
+      </c>
+      <c r="E812" t="s">
+        <v>13</v>
+      </c>
+      <c r="F812" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="813" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A813" t="s">
+        <v>10</v>
+      </c>
+      <c r="B813" t="s">
+        <v>11</v>
+      </c>
+      <c r="C813" t="s">
+        <v>0</v>
+      </c>
+      <c r="D813">
+        <v>4.8</v>
+      </c>
+      <c r="E813" t="s">
+        <v>13</v>
+      </c>
+      <c r="F813" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="814" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A814" t="s">
+        <v>2</v>
+      </c>
+      <c r="B814" t="s">
+        <v>11</v>
+      </c>
+      <c r="C814" t="s">
+        <v>0</v>
+      </c>
+      <c r="D814">
+        <v>7.6</v>
+      </c>
+      <c r="E814" t="s">
+        <v>13</v>
+      </c>
+      <c r="F814" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="815" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A815" t="s">
+        <v>2</v>
+      </c>
+      <c r="B815" t="s">
+        <v>11</v>
+      </c>
+      <c r="C815" t="s">
+        <v>0</v>
+      </c>
+      <c r="D815">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E815" t="s">
+        <v>13</v>
+      </c>
+      <c r="F815" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="816" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A816" t="s">
+        <v>2</v>
+      </c>
+      <c r="B816" t="s">
+        <v>11</v>
+      </c>
+      <c r="C816" t="s">
+        <v>0</v>
+      </c>
+      <c r="D816">
+        <v>3.1</v>
+      </c>
+      <c r="E816" t="s">
+        <v>13</v>
+      </c>
+      <c r="F816" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="817" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A817" t="s">
+        <v>2</v>
+      </c>
+      <c r="B817" t="s">
+        <v>11</v>
+      </c>
+      <c r="C817" t="s">
+        <v>0</v>
+      </c>
+      <c r="D817">
+        <v>7.3</v>
+      </c>
+      <c r="E817" t="s">
+        <v>13</v>
+      </c>
+      <c r="F817" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="818" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A818" t="s">
+        <v>2</v>
+      </c>
+      <c r="B818" t="s">
+        <v>11</v>
+      </c>
+      <c r="C818" t="s">
+        <v>0</v>
+      </c>
+      <c r="D818">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E818" t="s">
+        <v>13</v>
+      </c>
+      <c r="F818" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="819" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A819" t="s">
+        <v>2</v>
+      </c>
+      <c r="B819" t="s">
+        <v>11</v>
+      </c>
+      <c r="C819" t="s">
+        <v>0</v>
+      </c>
+      <c r="D819">
+        <v>2.9</v>
+      </c>
+      <c r="E819" t="s">
+        <v>13</v>
+      </c>
+      <c r="F819" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="820" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A820" t="s">
+        <v>2</v>
+      </c>
+      <c r="B820" t="s">
+        <v>11</v>
+      </c>
+      <c r="C820" t="s">
+        <v>0</v>
+      </c>
+      <c r="D820">
+        <v>15</v>
+      </c>
+      <c r="E820" t="s">
+        <v>13</v>
+      </c>
+      <c r="F820" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="821" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A821" t="s">
+        <v>2</v>
+      </c>
+      <c r="B821" t="s">
+        <v>11</v>
+      </c>
+      <c r="C821" t="s">
+        <v>0</v>
+      </c>
+      <c r="D821">
+        <v>8.1</v>
+      </c>
+      <c r="E821" t="s">
+        <v>13</v>
+      </c>
+      <c r="F821" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="822" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A822" t="s">
+        <v>2</v>
+      </c>
+      <c r="B822" t="s">
+        <v>11</v>
+      </c>
+      <c r="C822" t="s">
+        <v>0</v>
+      </c>
+      <c r="D822">
+        <v>17.2</v>
+      </c>
+      <c r="E822" t="s">
+        <v>13</v>
+      </c>
+      <c r="F822" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="823" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A823" t="s">
+        <v>2</v>
+      </c>
+      <c r="B823" t="s">
+        <v>11</v>
+      </c>
+      <c r="C823" t="s">
+        <v>0</v>
+      </c>
+      <c r="D823">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E823" t="s">
+        <v>13</v>
+      </c>
+      <c r="F823" s="1">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="824" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A824" t="s">
+        <v>10</v>
+      </c>
+      <c r="B824" t="s">
+        <v>8</v>
+      </c>
+      <c r="C824" t="s">
+        <v>0</v>
+      </c>
+      <c r="D824">
+        <v>1.7</v>
+      </c>
+      <c r="E824" t="s">
+        <v>13</v>
+      </c>
+      <c r="F824" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="825" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A825" t="s">
+        <v>10</v>
+      </c>
+      <c r="B825" t="s">
+        <v>8</v>
+      </c>
+      <c r="C825" t="s">
+        <v>0</v>
+      </c>
+      <c r="D825">
+        <v>2.6</v>
+      </c>
+      <c r="E825" t="s">
+        <v>13</v>
+      </c>
+      <c r="F825" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="826" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A826" t="s">
+        <v>10</v>
+      </c>
+      <c r="B826" t="s">
+        <v>8</v>
+      </c>
+      <c r="C826" t="s">
+        <v>0</v>
+      </c>
+      <c r="D826">
+        <v>5</v>
+      </c>
+      <c r="E826" t="s">
+        <v>13</v>
+      </c>
+      <c r="F826" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="827" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A827" t="s">
+        <v>10</v>
+      </c>
+      <c r="B827" t="s">
+        <v>8</v>
+      </c>
+      <c r="C827" t="s">
+        <v>0</v>
+      </c>
+      <c r="D827">
+        <v>3.3</v>
+      </c>
+      <c r="E827" t="s">
+        <v>13</v>
+      </c>
+      <c r="F827" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="828" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A828" t="s">
+        <v>10</v>
+      </c>
+      <c r="B828" t="s">
+        <v>8</v>
+      </c>
+      <c r="C828" t="s">
+        <v>0</v>
+      </c>
+      <c r="D828">
+        <v>7.8</v>
+      </c>
+      <c r="E828" t="s">
+        <v>13</v>
+      </c>
+      <c r="F828" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="829" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A829" t="s">
+        <v>10</v>
+      </c>
+      <c r="B829" t="s">
+        <v>8</v>
+      </c>
+      <c r="C829" t="s">
+        <v>0</v>
+      </c>
+      <c r="D829">
+        <v>4</v>
+      </c>
+      <c r="E829" t="s">
+        <v>13</v>
+      </c>
+      <c r="F829" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="830" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A830" t="s">
+        <v>10</v>
+      </c>
+      <c r="B830" t="s">
+        <v>8</v>
+      </c>
+      <c r="C830" t="s">
+        <v>0</v>
+      </c>
+      <c r="D830">
+        <v>4.2</v>
+      </c>
+      <c r="E830" t="s">
+        <v>13</v>
+      </c>
+      <c r="F830" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="831" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A831" t="s">
+        <v>10</v>
+      </c>
+      <c r="B831" t="s">
+        <v>8</v>
+      </c>
+      <c r="C831" t="s">
+        <v>0</v>
+      </c>
+      <c r="D831">
+        <v>7.1</v>
+      </c>
+      <c r="E831" t="s">
+        <v>13</v>
+      </c>
+      <c r="F831" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="832" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A832" t="s">
+        <v>10</v>
+      </c>
+      <c r="B832" t="s">
+        <v>8</v>
+      </c>
+      <c r="C832" t="s">
+        <v>0</v>
+      </c>
+      <c r="D832">
+        <v>2.1</v>
+      </c>
+      <c r="E832" t="s">
+        <v>13</v>
+      </c>
+      <c r="F832" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="833" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A833" t="s">
+        <v>10</v>
+      </c>
+      <c r="B833" t="s">
+        <v>8</v>
+      </c>
+      <c r="C833" t="s">
+        <v>0</v>
+      </c>
+      <c r="D833">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E833" t="s">
+        <v>13</v>
+      </c>
+      <c r="F833" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="834" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A834" t="s">
+        <v>10</v>
+      </c>
+      <c r="B834" t="s">
+        <v>8</v>
+      </c>
+      <c r="C834" t="s">
+        <v>0</v>
+      </c>
+      <c r="D834">
+        <v>2.8</v>
+      </c>
+      <c r="E834" t="s">
+        <v>13</v>
+      </c>
+      <c r="F834" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="835" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A835" t="s">
+        <v>10</v>
+      </c>
+      <c r="B835" t="s">
+        <v>8</v>
+      </c>
+      <c r="C835" t="s">
+        <v>0</v>
+      </c>
+      <c r="D835">
+        <v>5.7</v>
+      </c>
+      <c r="E835" t="s">
+        <v>13</v>
+      </c>
+      <c r="F835" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="836" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A836" t="s">
+        <v>10</v>
+      </c>
+      <c r="B836" t="s">
+        <v>8</v>
+      </c>
+      <c r="C836" t="s">
+        <v>0</v>
+      </c>
+      <c r="D836">
+        <v>5.7</v>
+      </c>
+      <c r="E836" t="s">
+        <v>13</v>
+      </c>
+      <c r="F836" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="837" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A837" t="s">
+        <v>10</v>
+      </c>
+      <c r="B837" t="s">
+        <v>8</v>
+      </c>
+      <c r="C837" t="s">
+        <v>0</v>
+      </c>
+      <c r="D837">
+        <v>8</v>
+      </c>
+      <c r="E837" t="s">
+        <v>13</v>
+      </c>
+      <c r="F837" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="838" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A838" t="s">
+        <v>2</v>
+      </c>
+      <c r="B838" t="s">
+        <v>8</v>
+      </c>
+      <c r="C838" t="s">
+        <v>0</v>
+      </c>
+      <c r="D838">
+        <v>4.2</v>
+      </c>
+      <c r="E838" t="s">
+        <v>13</v>
+      </c>
+      <c r="F838" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="839" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A839" t="s">
+        <v>2</v>
+      </c>
+      <c r="B839" t="s">
+        <v>8</v>
+      </c>
+      <c r="C839" t="s">
+        <v>0</v>
+      </c>
+      <c r="D839">
+        <v>6.4</v>
+      </c>
+      <c r="E839" t="s">
+        <v>13</v>
+      </c>
+      <c r="F839" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="840" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A840" t="s">
+        <v>2</v>
+      </c>
+      <c r="B840" t="s">
+        <v>8</v>
+      </c>
+      <c r="C840" t="s">
+        <v>0</v>
+      </c>
+      <c r="D840">
+        <v>2.1</v>
+      </c>
+      <c r="E840" t="s">
+        <v>13</v>
+      </c>
+      <c r="F840" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="841" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A841" t="s">
+        <v>2</v>
+      </c>
+      <c r="B841" t="s">
+        <v>8</v>
+      </c>
+      <c r="C841" t="s">
+        <v>0</v>
+      </c>
+      <c r="D841">
+        <v>5.2</v>
+      </c>
+      <c r="E841" t="s">
+        <v>13</v>
+      </c>
+      <c r="F841" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="842" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A842" t="s">
+        <v>2</v>
+      </c>
+      <c r="B842" t="s">
+        <v>8</v>
+      </c>
+      <c r="C842" t="s">
+        <v>0</v>
+      </c>
+      <c r="D842">
+        <v>7.9</v>
+      </c>
+      <c r="E842" t="s">
+        <v>13</v>
+      </c>
+      <c r="F842" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="843" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A843" t="s">
+        <v>2</v>
+      </c>
+      <c r="B843" t="s">
+        <v>8</v>
+      </c>
+      <c r="C843" t="s">
+        <v>0</v>
+      </c>
+      <c r="D843">
+        <v>6.7</v>
+      </c>
+      <c r="E843" t="s">
+        <v>13</v>
+      </c>
+      <c r="F843" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="844" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A844" t="s">
+        <v>2</v>
+      </c>
+      <c r="B844" t="s">
+        <v>8</v>
+      </c>
+      <c r="C844" t="s">
+        <v>0</v>
+      </c>
+      <c r="D844">
+        <v>3.6</v>
+      </c>
+      <c r="E844" t="s">
+        <v>13</v>
+      </c>
+      <c r="F844" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="845" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A845" t="s">
+        <v>2</v>
+      </c>
+      <c r="B845" t="s">
+        <v>8</v>
+      </c>
+      <c r="C845" t="s">
+        <v>0</v>
+      </c>
+      <c r="D845">
+        <v>3.3</v>
+      </c>
+      <c r="E845" t="s">
+        <v>13</v>
+      </c>
+      <c r="F845" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="846" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A846" t="s">
+        <v>2</v>
+      </c>
+      <c r="B846" t="s">
+        <v>8</v>
+      </c>
+      <c r="C846" t="s">
+        <v>0</v>
+      </c>
+      <c r="D846">
+        <v>2.9</v>
+      </c>
+      <c r="E846" t="s">
+        <v>13</v>
+      </c>
+      <c r="F846" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="847" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A847" t="s">
+        <v>2</v>
+      </c>
+      <c r="B847" t="s">
+        <v>8</v>
+      </c>
+      <c r="C847" t="s">
+        <v>0</v>
+      </c>
+      <c r="D847">
+        <v>2.9</v>
+      </c>
+      <c r="E847" t="s">
+        <v>13</v>
+      </c>
+      <c r="F847" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="848" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A848" t="s">
+        <v>2</v>
+      </c>
+      <c r="B848" t="s">
+        <v>8</v>
+      </c>
+      <c r="C848" t="s">
+        <v>0</v>
+      </c>
+      <c r="D848">
+        <v>4.2</v>
+      </c>
+      <c r="E848" t="s">
+        <v>13</v>
+      </c>
+      <c r="F848" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="849" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A849" t="s">
+        <v>2</v>
+      </c>
+      <c r="B849" t="s">
+        <v>8</v>
+      </c>
+      <c r="C849" t="s">
+        <v>0</v>
+      </c>
+      <c r="D849">
+        <v>6.1</v>
+      </c>
+      <c r="E849" t="s">
+        <v>13</v>
+      </c>
+      <c r="F849" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="850" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A850" t="s">
+        <v>2</v>
+      </c>
+      <c r="B850" t="s">
+        <v>8</v>
+      </c>
+      <c r="C850" t="s">
+        <v>0</v>
+      </c>
+      <c r="D850">
+        <v>5.6</v>
+      </c>
+      <c r="E850" t="s">
+        <v>13</v>
+      </c>
+      <c r="F850" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="851" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A851" t="s">
+        <v>2</v>
+      </c>
+      <c r="B851" t="s">
+        <v>8</v>
+      </c>
+      <c r="C851" t="s">
+        <v>0</v>
+      </c>
+      <c r="D851">
+        <v>4</v>
+      </c>
+      <c r="E851" t="s">
+        <v>13</v>
+      </c>
+      <c r="F851" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="852" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A852" t="s">
+        <v>2</v>
+      </c>
+      <c r="B852" t="s">
+        <v>8</v>
+      </c>
+      <c r="C852" t="s">
+        <v>0</v>
+      </c>
+      <c r="D852">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E852" t="s">
+        <v>13</v>
+      </c>
+      <c r="F852" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="853" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A853" t="s">
+        <v>2</v>
+      </c>
+      <c r="B853" t="s">
+        <v>8</v>
+      </c>
+      <c r="C853" t="s">
+        <v>0</v>
+      </c>
+      <c r="D853">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E853" t="s">
+        <v>13</v>
+      </c>
+      <c r="F853" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="854" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A854" t="s">
+        <v>10</v>
+      </c>
+      <c r="B854" t="s">
+        <v>11</v>
+      </c>
+      <c r="C854" t="s">
+        <v>0</v>
+      </c>
+      <c r="D854">
+        <v>4.2</v>
+      </c>
+      <c r="E854" t="s">
+        <v>13</v>
+      </c>
+      <c r="F854" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="855" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A855" t="s">
+        <v>10</v>
+      </c>
+      <c r="B855" t="s">
+        <v>11</v>
+      </c>
+      <c r="C855" t="s">
+        <v>0</v>
+      </c>
+      <c r="D855">
+        <v>6.9</v>
+      </c>
+      <c r="E855" t="s">
+        <v>13</v>
+      </c>
+      <c r="F855" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="856" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A856" t="s">
+        <v>10</v>
+      </c>
+      <c r="B856" t="s">
+        <v>11</v>
+      </c>
+      <c r="C856" t="s">
+        <v>0</v>
+      </c>
+      <c r="D856">
+        <v>6.9</v>
+      </c>
+      <c r="E856" t="s">
+        <v>13</v>
+      </c>
+      <c r="F856" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="857" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A857" t="s">
+        <v>10</v>
+      </c>
+      <c r="B857" t="s">
+        <v>11</v>
+      </c>
+      <c r="C857" t="s">
+        <v>0</v>
+      </c>
+      <c r="D857">
+        <v>7.3</v>
+      </c>
+      <c r="E857" t="s">
+        <v>13</v>
+      </c>
+      <c r="F857" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="858" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A858" t="s">
+        <v>10</v>
+      </c>
+      <c r="B858" t="s">
+        <v>11</v>
+      </c>
+      <c r="C858" t="s">
+        <v>0</v>
+      </c>
+      <c r="D858">
+        <v>5.2</v>
+      </c>
+      <c r="E858" t="s">
+        <v>13</v>
+      </c>
+      <c r="F858" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="859" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A859" t="s">
+        <v>10</v>
+      </c>
+      <c r="B859" t="s">
+        <v>11</v>
+      </c>
+      <c r="C859" t="s">
+        <v>0</v>
+      </c>
+      <c r="D859">
+        <v>5.8</v>
+      </c>
+      <c r="E859" t="s">
+        <v>13</v>
+      </c>
+      <c r="F859" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="860" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A860" t="s">
+        <v>10</v>
+      </c>
+      <c r="B860" t="s">
+        <v>11</v>
+      </c>
+      <c r="C860" t="s">
+        <v>0</v>
+      </c>
+      <c r="D860">
+        <v>11.7</v>
+      </c>
+      <c r="E860" t="s">
+        <v>13</v>
+      </c>
+      <c r="F860" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="861" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A861" t="s">
+        <v>10</v>
+      </c>
+      <c r="B861" t="s">
+        <v>11</v>
+      </c>
+      <c r="C861" t="s">
+        <v>0</v>
+      </c>
+      <c r="D861">
+        <v>16.3</v>
+      </c>
+      <c r="E861" t="s">
+        <v>13</v>
+      </c>
+      <c r="F861" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="862" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A862" t="s">
+        <v>10</v>
+      </c>
+      <c r="B862" t="s">
+        <v>11</v>
+      </c>
+      <c r="C862" t="s">
+        <v>0</v>
+      </c>
+      <c r="D862">
+        <v>5</v>
+      </c>
+      <c r="E862" t="s">
+        <v>13</v>
+      </c>
+      <c r="F862" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="863" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A863" t="s">
+        <v>10</v>
+      </c>
+      <c r="B863" t="s">
+        <v>11</v>
+      </c>
+      <c r="C863" t="s">
+        <v>0</v>
+      </c>
+      <c r="D863">
+        <v>10.6</v>
+      </c>
+      <c r="E863" t="s">
+        <v>13</v>
+      </c>
+      <c r="F863" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="864" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A864" t="s">
+        <v>10</v>
+      </c>
+      <c r="B864" t="s">
+        <v>11</v>
+      </c>
+      <c r="C864" t="s">
+        <v>0</v>
+      </c>
+      <c r="D864">
+        <v>3.5</v>
+      </c>
+      <c r="E864" t="s">
+        <v>13</v>
+      </c>
+      <c r="F864" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A865" t="s">
+        <v>10</v>
+      </c>
+      <c r="B865" t="s">
+        <v>11</v>
+      </c>
+      <c r="C865" t="s">
+        <v>0</v>
+      </c>
+      <c r="D865">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E865" t="s">
+        <v>13</v>
+      </c>
+      <c r="F865" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A866" t="s">
+        <v>2</v>
+      </c>
+      <c r="B866" t="s">
+        <v>11</v>
+      </c>
+      <c r="C866" t="s">
+        <v>0</v>
+      </c>
+      <c r="D866">
+        <v>2.8</v>
+      </c>
+      <c r="E866" t="s">
+        <v>13</v>
+      </c>
+      <c r="F866" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A867" t="s">
+        <v>2</v>
+      </c>
+      <c r="B867" t="s">
+        <v>11</v>
+      </c>
+      <c r="C867" t="s">
+        <v>0</v>
+      </c>
+      <c r="D867">
+        <v>7.8</v>
+      </c>
+      <c r="E867" t="s">
+        <v>13</v>
+      </c>
+      <c r="F867" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A868" t="s">
+        <v>2</v>
+      </c>
+      <c r="B868" t="s">
+        <v>11</v>
+      </c>
+      <c r="C868" t="s">
+        <v>0</v>
+      </c>
+      <c r="D868">
+        <v>7.3</v>
+      </c>
+      <c r="E868" t="s">
+        <v>13</v>
+      </c>
+      <c r="F868" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A869" t="s">
+        <v>2</v>
+      </c>
+      <c r="B869" t="s">
+        <v>11</v>
+      </c>
+      <c r="C869" t="s">
+        <v>0</v>
+      </c>
+      <c r="D869">
+        <v>3.8</v>
+      </c>
+      <c r="E869" t="s">
+        <v>13</v>
+      </c>
+      <c r="F869" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="870" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A870" t="s">
+        <v>2</v>
+      </c>
+      <c r="B870" t="s">
+        <v>11</v>
+      </c>
+      <c r="C870" t="s">
+        <v>0</v>
+      </c>
+      <c r="D870">
+        <v>2.9</v>
+      </c>
+      <c r="E870" t="s">
+        <v>13</v>
+      </c>
+      <c r="F870" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="871" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A871" t="s">
+        <v>2</v>
+      </c>
+      <c r="B871" t="s">
+        <v>11</v>
+      </c>
+      <c r="C871" t="s">
+        <v>0</v>
+      </c>
+      <c r="D871">
+        <v>11</v>
+      </c>
+      <c r="E871" t="s">
+        <v>13</v>
+      </c>
+      <c r="F871" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="872" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A872" t="s">
+        <v>2</v>
+      </c>
+      <c r="B872" t="s">
+        <v>11</v>
+      </c>
+      <c r="C872" t="s">
+        <v>0</v>
+      </c>
+      <c r="D872">
+        <v>2.7</v>
+      </c>
+      <c r="E872" t="s">
+        <v>13</v>
+      </c>
+      <c r="F872" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="873" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A873" t="s">
+        <v>2</v>
+      </c>
+      <c r="B873" t="s">
+        <v>11</v>
+      </c>
+      <c r="C873" t="s">
+        <v>0</v>
+      </c>
+      <c r="D873">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E873" t="s">
+        <v>13</v>
+      </c>
+      <c r="F873" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="874" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A874" t="s">
+        <v>2</v>
+      </c>
+      <c r="B874" t="s">
+        <v>11</v>
+      </c>
+      <c r="C874" t="s">
+        <v>0</v>
+      </c>
+      <c r="D874">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E874" t="s">
+        <v>13</v>
+      </c>
+      <c r="F874" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="875" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A875" t="s">
+        <v>2</v>
+      </c>
+      <c r="B875" t="s">
+        <v>11</v>
+      </c>
+      <c r="C875" t="s">
+        <v>0</v>
+      </c>
+      <c r="D875">
+        <v>3.6</v>
+      </c>
+      <c r="E875" t="s">
+        <v>13</v>
+      </c>
+      <c r="F875" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="876" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A876" t="s">
+        <v>2</v>
+      </c>
+      <c r="B876" t="s">
+        <v>11</v>
+      </c>
+      <c r="C876" t="s">
+        <v>0</v>
+      </c>
+      <c r="D876">
+        <v>7.2</v>
+      </c>
+      <c r="E876" t="s">
+        <v>13</v>
+      </c>
+      <c r="F876" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="877" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A877" t="s">
+        <v>2</v>
+      </c>
+      <c r="B877" t="s">
+        <v>11</v>
+      </c>
+      <c r="C877" t="s">
+        <v>0</v>
+      </c>
+      <c r="D877">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E877" t="s">
+        <v>13</v>
+      </c>
+      <c r="F877" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="878" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A878" t="s">
+        <v>2</v>
+      </c>
+      <c r="B878" t="s">
+        <v>11</v>
+      </c>
+      <c r="C878" t="s">
+        <v>0</v>
+      </c>
+      <c r="D878">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E878" t="s">
+        <v>13</v>
+      </c>
+      <c r="F878" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="879" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A879" t="s">
+        <v>2</v>
+      </c>
+      <c r="B879" t="s">
+        <v>11</v>
+      </c>
+      <c r="C879" t="s">
+        <v>0</v>
+      </c>
+      <c r="D879">
+        <v>14.1</v>
+      </c>
+      <c r="E879" t="s">
+        <v>13</v>
+      </c>
+      <c r="F879" s="1">
+        <v>44838</v>
+      </c>
+    </row>
+    <row r="880" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A880" t="s">
+        <v>10</v>
+      </c>
+      <c r="B880" t="s">
+        <v>8</v>
+      </c>
+      <c r="C880" t="s">
+        <v>0</v>
+      </c>
+      <c r="D880">
+        <v>11.79</v>
+      </c>
+      <c r="E880" t="s">
+        <v>1</v>
+      </c>
+      <c r="F880" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="881" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A881" t="s">
+        <v>10</v>
+      </c>
+      <c r="B881" t="s">
+        <v>8</v>
+      </c>
+      <c r="C881" t="s">
+        <v>0</v>
+      </c>
+      <c r="D881">
+        <v>3.58</v>
+      </c>
+      <c r="E881" t="s">
+        <v>1</v>
+      </c>
+      <c r="F881" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="882" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A882" t="s">
+        <v>10</v>
+      </c>
+      <c r="B882" t="s">
+        <v>8</v>
+      </c>
+      <c r="C882" t="s">
+        <v>0</v>
+      </c>
+      <c r="D882">
+        <v>4.59</v>
+      </c>
+      <c r="E882" t="s">
+        <v>1</v>
+      </c>
+      <c r="F882" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="883" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A883" t="s">
+        <v>10</v>
+      </c>
+      <c r="B883" t="s">
+        <v>8</v>
+      </c>
+      <c r="C883" t="s">
+        <v>0</v>
+      </c>
+      <c r="D883">
+        <v>4.08</v>
+      </c>
+      <c r="E883" t="s">
+        <v>1</v>
+      </c>
+      <c r="F883" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="884" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A884" t="s">
+        <v>10</v>
+      </c>
+      <c r="B884" t="s">
+        <v>8</v>
+      </c>
+      <c r="C884" t="s">
+        <v>0</v>
+      </c>
+      <c r="D884">
+        <v>6.84</v>
+      </c>
+      <c r="E884" t="s">
+        <v>1</v>
+      </c>
+      <c r="F884" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="885" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A885" t="s">
+        <v>10</v>
+      </c>
+      <c r="B885" t="s">
+        <v>8</v>
+      </c>
+      <c r="C885" t="s">
+        <v>0</v>
+      </c>
+      <c r="D885">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E885" t="s">
+        <v>1</v>
+      </c>
+      <c r="F885" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="886" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A886" t="s">
+        <v>10</v>
+      </c>
+      <c r="B886" t="s">
+        <v>8</v>
+      </c>
+      <c r="C886" t="s">
+        <v>0</v>
+      </c>
+      <c r="D886">
+        <v>3.02</v>
+      </c>
+      <c r="E886" t="s">
+        <v>1</v>
+      </c>
+      <c r="F886" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="887" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A887" t="s">
+        <v>10</v>
+      </c>
+      <c r="B887" t="s">
+        <v>8</v>
+      </c>
+      <c r="C887" t="s">
+        <v>0</v>
+      </c>
+      <c r="D887">
+        <v>2.27</v>
+      </c>
+      <c r="E887" t="s">
+        <v>1</v>
+      </c>
+      <c r="F887" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="888" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A888" t="s">
+        <v>10</v>
+      </c>
+      <c r="B888" t="s">
+        <v>8</v>
+      </c>
+      <c r="C888" t="s">
+        <v>0</v>
+      </c>
+      <c r="D888">
+        <v>3.58</v>
+      </c>
+      <c r="E888" t="s">
+        <v>1</v>
+      </c>
+      <c r="F888" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A889" t="s">
+        <v>10</v>
+      </c>
+      <c r="B889" t="s">
+        <v>8</v>
+      </c>
+      <c r="C889" t="s">
+        <v>0</v>
+      </c>
+      <c r="D889">
+        <v>3.06</v>
+      </c>
+      <c r="E889" t="s">
+        <v>1</v>
+      </c>
+      <c r="F889" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="890" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A890" t="s">
+        <v>10</v>
+      </c>
+      <c r="B890" t="s">
+        <v>8</v>
+      </c>
+      <c r="C890" t="s">
+        <v>0</v>
+      </c>
+      <c r="D890">
+        <v>4.08</v>
+      </c>
+      <c r="E890" t="s">
+        <v>1</v>
+      </c>
+      <c r="F890" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="891" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A891" t="s">
+        <v>10</v>
+      </c>
+      <c r="B891" t="s">
+        <v>8</v>
+      </c>
+      <c r="C891" t="s">
+        <v>0</v>
+      </c>
+      <c r="D891">
+        <v>3.95</v>
+      </c>
+      <c r="E891" t="s">
+        <v>1</v>
+      </c>
+      <c r="F891" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="892" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A892" t="s">
+        <v>10</v>
+      </c>
+      <c r="B892" t="s">
+        <v>8</v>
+      </c>
+      <c r="C892" t="s">
+        <v>0</v>
+      </c>
+      <c r="D892">
+        <v>15.38</v>
+      </c>
+      <c r="E892" t="s">
+        <v>1</v>
+      </c>
+      <c r="F892" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A893" t="s">
+        <v>10</v>
+      </c>
+      <c r="B893" t="s">
+        <v>8</v>
+      </c>
+      <c r="C893" t="s">
+        <v>0</v>
+      </c>
+      <c r="D893">
+        <v>8.26</v>
+      </c>
+      <c r="E893" t="s">
+        <v>1</v>
+      </c>
+      <c r="F893" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="894" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A894" t="s">
+        <v>10</v>
+      </c>
+      <c r="B894" t="s">
+        <v>8</v>
+      </c>
+      <c r="C894" t="s">
+        <v>0</v>
+      </c>
+      <c r="D894">
+        <v>4.22</v>
+      </c>
+      <c r="E894" t="s">
+        <v>1</v>
+      </c>
+      <c r="F894" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="895" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A895" t="s">
+        <v>10</v>
+      </c>
+      <c r="B895" t="s">
+        <v>8</v>
+      </c>
+      <c r="C895" t="s">
+        <v>0</v>
+      </c>
+      <c r="D895">
+        <v>5.32</v>
+      </c>
+      <c r="E895" t="s">
+        <v>1</v>
+      </c>
+      <c r="F895" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A896" t="s">
+        <v>10</v>
+      </c>
+      <c r="B896" t="s">
+        <v>8</v>
+      </c>
+      <c r="C896" t="s">
+        <v>0</v>
+      </c>
+      <c r="D896">
+        <v>10.28</v>
+      </c>
+      <c r="E896" t="s">
+        <v>1</v>
+      </c>
+      <c r="F896" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A897" t="s">
+        <v>10</v>
+      </c>
+      <c r="B897" t="s">
+        <v>8</v>
+      </c>
+      <c r="C897" t="s">
+        <v>0</v>
+      </c>
+      <c r="D897">
+        <v>8.64</v>
+      </c>
+      <c r="E897" t="s">
+        <v>1</v>
+      </c>
+      <c r="F897" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="898" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A898" t="s">
+        <v>10</v>
+      </c>
+      <c r="B898" t="s">
+        <v>8</v>
+      </c>
+      <c r="C898" t="s">
+        <v>0</v>
+      </c>
+      <c r="D898">
+        <v>7.42</v>
+      </c>
+      <c r="E898" t="s">
+        <v>1</v>
+      </c>
+      <c r="F898" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="899" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A899" t="s">
+        <v>10</v>
+      </c>
+      <c r="B899" t="s">
+        <v>8</v>
+      </c>
+      <c r="C899" t="s">
+        <v>0</v>
+      </c>
+      <c r="D899">
+        <v>6.02</v>
+      </c>
+      <c r="E899" t="s">
+        <v>1</v>
+      </c>
+      <c r="F899" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="900" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A900" t="s">
+        <v>2</v>
+      </c>
+      <c r="B900" t="s">
+        <v>8</v>
+      </c>
+      <c r="C900" t="s">
+        <v>0</v>
+      </c>
+      <c r="D900">
+        <v>5.37</v>
+      </c>
+      <c r="E900" t="s">
+        <v>1</v>
+      </c>
+      <c r="F900" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="901" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A901" t="s">
+        <v>2</v>
+      </c>
+      <c r="B901" t="s">
+        <v>8</v>
+      </c>
+      <c r="C901" t="s">
+        <v>0</v>
+      </c>
+      <c r="D901">
+        <v>8.19</v>
+      </c>
+      <c r="E901" t="s">
+        <v>1</v>
+      </c>
+      <c r="F901" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="902" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A902" t="s">
+        <v>2</v>
+      </c>
+      <c r="B902" t="s">
+        <v>8</v>
+      </c>
+      <c r="C902" t="s">
+        <v>0</v>
+      </c>
+      <c r="D902">
+        <v>4.54</v>
+      </c>
+      <c r="E902" t="s">
+        <v>1</v>
+      </c>
+      <c r="F902" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A903" t="s">
+        <v>2</v>
+      </c>
+      <c r="B903" t="s">
+        <v>8</v>
+      </c>
+      <c r="C903" t="s">
+        <v>0</v>
+      </c>
+      <c r="D903">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E903" t="s">
+        <v>1</v>
+      </c>
+      <c r="F903" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A904" t="s">
+        <v>2</v>
+      </c>
+      <c r="B904" t="s">
+        <v>8</v>
+      </c>
+      <c r="C904" t="s">
+        <v>0</v>
+      </c>
+      <c r="D904">
+        <v>6.39</v>
+      </c>
+      <c r="E904" t="s">
+        <v>1</v>
+      </c>
+      <c r="F904" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="905" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A905" t="s">
+        <v>2</v>
+      </c>
+      <c r="B905" t="s">
+        <v>8</v>
+      </c>
+      <c r="C905" t="s">
+        <v>0</v>
+      </c>
+      <c r="D905">
+        <v>5.17</v>
+      </c>
+      <c r="E905" t="s">
+        <v>1</v>
+      </c>
+      <c r="F905" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="906" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A906" t="s">
+        <v>2</v>
+      </c>
+      <c r="B906" t="s">
+        <v>8</v>
+      </c>
+      <c r="C906" t="s">
+        <v>0</v>
+      </c>
+      <c r="D906">
+        <v>7.47</v>
+      </c>
+      <c r="E906" t="s">
+        <v>1</v>
+      </c>
+      <c r="F906" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="907" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A907" t="s">
+        <v>2</v>
+      </c>
+      <c r="B907" t="s">
+        <v>8</v>
+      </c>
+      <c r="C907" t="s">
+        <v>0</v>
+      </c>
+      <c r="D907">
+        <v>13.15</v>
+      </c>
+      <c r="E907" t="s">
+        <v>1</v>
+      </c>
+      <c r="F907" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A908" t="s">
+        <v>2</v>
+      </c>
+      <c r="B908" t="s">
+        <v>8</v>
+      </c>
+      <c r="C908" t="s">
+        <v>0</v>
+      </c>
+      <c r="D908">
+        <v>6.12</v>
+      </c>
+      <c r="E908" t="s">
+        <v>1</v>
+      </c>
+      <c r="F908" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="909" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A909" t="s">
+        <v>2</v>
+      </c>
+      <c r="B909" t="s">
+        <v>8</v>
+      </c>
+      <c r="C909" t="s">
+        <v>0</v>
+      </c>
+      <c r="D909">
+        <v>11.03</v>
+      </c>
+      <c r="E909" t="s">
+        <v>1</v>
+      </c>
+      <c r="F909" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="910" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A910" t="s">
+        <v>2</v>
+      </c>
+      <c r="B910" t="s">
+        <v>8</v>
+      </c>
+      <c r="C910" t="s">
+        <v>0</v>
+      </c>
+      <c r="D910">
+        <v>2.9</v>
+      </c>
+      <c r="E910" t="s">
+        <v>1</v>
+      </c>
+      <c r="F910" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="911" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A911" t="s">
+        <v>2</v>
+      </c>
+      <c r="B911" t="s">
+        <v>8</v>
+      </c>
+      <c r="C911" t="s">
+        <v>0</v>
+      </c>
+      <c r="D911">
+        <v>7.68</v>
+      </c>
+      <c r="E911" t="s">
+        <v>1</v>
+      </c>
+      <c r="F911" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A912" t="s">
+        <v>2</v>
+      </c>
+      <c r="B912" t="s">
+        <v>8</v>
+      </c>
+      <c r="C912" t="s">
+        <v>0</v>
+      </c>
+      <c r="D912">
+        <v>10.81</v>
+      </c>
+      <c r="E912" t="s">
+        <v>1</v>
+      </c>
+      <c r="F912" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="913" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A913" t="s">
+        <v>2</v>
+      </c>
+      <c r="B913" t="s">
+        <v>8</v>
+      </c>
+      <c r="C913" t="s">
+        <v>0</v>
+      </c>
+      <c r="D913">
+        <v>3.03</v>
+      </c>
+      <c r="E913" t="s">
+        <v>1</v>
+      </c>
+      <c r="F913" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="914" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A914" t="s">
+        <v>2</v>
+      </c>
+      <c r="B914" t="s">
+        <v>8</v>
+      </c>
+      <c r="C914" t="s">
+        <v>0</v>
+      </c>
+      <c r="D914">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="E914" t="s">
+        <v>1</v>
+      </c>
+      <c r="F914" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="915" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A915" t="s">
+        <v>2</v>
+      </c>
+      <c r="B915" t="s">
+        <v>8</v>
+      </c>
+      <c r="C915" t="s">
+        <v>0</v>
+      </c>
+      <c r="D915">
+        <v>8.92</v>
+      </c>
+      <c r="E915" t="s">
+        <v>1</v>
+      </c>
+      <c r="F915" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="916" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A916" t="s">
+        <v>2</v>
+      </c>
+      <c r="B916" t="s">
+        <v>8</v>
+      </c>
+      <c r="C916" t="s">
+        <v>0</v>
+      </c>
+      <c r="D916">
+        <v>11.92</v>
+      </c>
+      <c r="E916" t="s">
+        <v>1</v>
+      </c>
+      <c r="F916" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="917" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A917" t="s">
+        <v>2</v>
+      </c>
+      <c r="B917" t="s">
+        <v>8</v>
+      </c>
+      <c r="C917" t="s">
+        <v>0</v>
+      </c>
+      <c r="D917">
+        <v>14.53</v>
+      </c>
+      <c r="E917" t="s">
+        <v>1</v>
+      </c>
+      <c r="F917" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="918" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A918" t="s">
+        <v>2</v>
+      </c>
+      <c r="B918" t="s">
+        <v>8</v>
+      </c>
+      <c r="C918" t="s">
+        <v>0</v>
+      </c>
+      <c r="D918">
+        <v>11.86</v>
+      </c>
+      <c r="E918" t="s">
+        <v>1</v>
+      </c>
+      <c r="F918" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="919" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A919" t="s">
+        <v>10</v>
+      </c>
+      <c r="B919" t="s">
+        <v>11</v>
+      </c>
+      <c r="C919" t="s">
+        <v>0</v>
+      </c>
+      <c r="D919">
+        <v>8.69</v>
+      </c>
+      <c r="E919" t="s">
+        <v>1</v>
+      </c>
+      <c r="F919" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="920" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A920" t="s">
+        <v>10</v>
+      </c>
+      <c r="B920" t="s">
+        <v>11</v>
+      </c>
+      <c r="C920" t="s">
+        <v>0</v>
+      </c>
+      <c r="D920">
+        <v>7.79</v>
+      </c>
+      <c r="E920" t="s">
+        <v>1</v>
+      </c>
+      <c r="F920" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="921" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A921" t="s">
+        <v>10</v>
+      </c>
+      <c r="B921" t="s">
+        <v>11</v>
+      </c>
+      <c r="C921" t="s">
+        <v>0</v>
+      </c>
+      <c r="D921">
+        <v>5.21</v>
+      </c>
+      <c r="E921" t="s">
+        <v>1</v>
+      </c>
+      <c r="F921" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="922" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A922" t="s">
+        <v>10</v>
+      </c>
+      <c r="B922" t="s">
+        <v>11</v>
+      </c>
+      <c r="C922" t="s">
+        <v>0</v>
+      </c>
+      <c r="D922">
+        <v>5.85</v>
+      </c>
+      <c r="E922" t="s">
+        <v>1</v>
+      </c>
+      <c r="F922" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="923" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A923" t="s">
+        <v>10</v>
+      </c>
+      <c r="B923" t="s">
+        <v>11</v>
+      </c>
+      <c r="C923" t="s">
+        <v>0</v>
+      </c>
+      <c r="D923">
+        <v>10.36</v>
+      </c>
+      <c r="E923" t="s">
+        <v>1</v>
+      </c>
+      <c r="F923" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="924" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A924" t="s">
+        <v>10</v>
+      </c>
+      <c r="B924" t="s">
+        <v>11</v>
+      </c>
+      <c r="C924" t="s">
+        <v>0</v>
+      </c>
+      <c r="D924">
+        <v>16.87</v>
+      </c>
+      <c r="E924" t="s">
+        <v>1</v>
+      </c>
+      <c r="F924" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="925" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A925" t="s">
+        <v>10</v>
+      </c>
+      <c r="B925" t="s">
+        <v>11</v>
+      </c>
+      <c r="C925" t="s">
+        <v>0</v>
+      </c>
+      <c r="D925">
+        <v>3.52</v>
+      </c>
+      <c r="E925" t="s">
+        <v>1</v>
+      </c>
+      <c r="F925" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="926" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A926" t="s">
+        <v>10</v>
+      </c>
+      <c r="B926" t="s">
+        <v>11</v>
+      </c>
+      <c r="C926" t="s">
+        <v>0</v>
+      </c>
+      <c r="D926">
+        <v>15.82</v>
+      </c>
+      <c r="E926" t="s">
+        <v>1</v>
+      </c>
+      <c r="F926" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="927" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A927" t="s">
+        <v>10</v>
+      </c>
+      <c r="B927" t="s">
+        <v>11</v>
+      </c>
+      <c r="C927" t="s">
+        <v>0</v>
+      </c>
+      <c r="D927">
+        <v>15.91</v>
+      </c>
+      <c r="E927" t="s">
+        <v>1</v>
+      </c>
+      <c r="F927" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="928" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A928" t="s">
+        <v>10</v>
+      </c>
+      <c r="B928" t="s">
+        <v>11</v>
+      </c>
+      <c r="C928" t="s">
+        <v>0</v>
+      </c>
+      <c r="D928">
+        <v>18.39</v>
+      </c>
+      <c r="E928" t="s">
+        <v>1</v>
+      </c>
+      <c r="F928" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="929" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A929" t="s">
+        <v>10</v>
+      </c>
+      <c r="B929" t="s">
+        <v>11</v>
+      </c>
+      <c r="C929" t="s">
+        <v>0</v>
+      </c>
+      <c r="D929">
+        <v>9.84</v>
+      </c>
+      <c r="E929" t="s">
+        <v>1</v>
+      </c>
+      <c r="F929" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="930" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A930" t="s">
+        <v>10</v>
+      </c>
+      <c r="B930" t="s">
+        <v>11</v>
+      </c>
+      <c r="C930" t="s">
+        <v>0</v>
+      </c>
+      <c r="D930">
+        <v>3.09</v>
+      </c>
+      <c r="E930" t="s">
+        <v>1</v>
+      </c>
+      <c r="F930" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="931" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A931" t="s">
+        <v>10</v>
+      </c>
+      <c r="B931" t="s">
+        <v>11</v>
+      </c>
+      <c r="C931" t="s">
+        <v>0</v>
+      </c>
+      <c r="D931">
+        <v>14.39</v>
+      </c>
+      <c r="E931" t="s">
+        <v>1</v>
+      </c>
+      <c r="F931" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="932" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A932" t="s">
+        <v>10</v>
+      </c>
+      <c r="B932" t="s">
+        <v>11</v>
+      </c>
+      <c r="C932" t="s">
+        <v>0</v>
+      </c>
+      <c r="D932">
+        <v>5.28</v>
+      </c>
+      <c r="E932" t="s">
+        <v>1</v>
+      </c>
+      <c r="F932" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="933" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A933" t="s">
+        <v>2</v>
+      </c>
+      <c r="B933" t="s">
+        <v>11</v>
+      </c>
+      <c r="C933" t="s">
+        <v>0</v>
+      </c>
+      <c r="D933">
+        <v>4.53</v>
+      </c>
+      <c r="E933" t="s">
+        <v>1</v>
+      </c>
+      <c r="F933" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="934" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A934" t="s">
+        <v>2</v>
+      </c>
+      <c r="B934" t="s">
+        <v>11</v>
+      </c>
+      <c r="C934" t="s">
+        <v>0</v>
+      </c>
+      <c r="D934">
+        <v>13.29</v>
+      </c>
+      <c r="E934" t="s">
+        <v>1</v>
+      </c>
+      <c r="F934" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="935" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A935" t="s">
+        <v>2</v>
+      </c>
+      <c r="B935" t="s">
+        <v>11</v>
+      </c>
+      <c r="C935" t="s">
+        <v>0</v>
+      </c>
+      <c r="D935">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="E935" t="s">
+        <v>1</v>
+      </c>
+      <c r="F935" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="936" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A936" t="s">
+        <v>2</v>
+      </c>
+      <c r="B936" t="s">
+        <v>11</v>
+      </c>
+      <c r="C936" t="s">
+        <v>0</v>
+      </c>
+      <c r="D936">
+        <v>9.26</v>
+      </c>
+      <c r="E936" t="s">
+        <v>1</v>
+      </c>
+      <c r="F936" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="937" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A937" t="s">
+        <v>2</v>
+      </c>
+      <c r="B937" t="s">
+        <v>11</v>
+      </c>
+      <c r="C937" t="s">
+        <v>0</v>
+      </c>
+      <c r="D937">
+        <v>12.76</v>
+      </c>
+      <c r="E937" t="s">
+        <v>1</v>
+      </c>
+      <c r="F937" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="938" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A938" t="s">
+        <v>2</v>
+      </c>
+      <c r="B938" t="s">
+        <v>11</v>
+      </c>
+      <c r="C938" t="s">
+        <v>0</v>
+      </c>
+      <c r="D938">
+        <v>3.37</v>
+      </c>
+      <c r="E938" t="s">
+        <v>1</v>
+      </c>
+      <c r="F938" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="939" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A939" t="s">
+        <v>2</v>
+      </c>
+      <c r="B939" t="s">
+        <v>11</v>
+      </c>
+      <c r="C939" t="s">
+        <v>0</v>
+      </c>
+      <c r="D939">
+        <v>9.19</v>
+      </c>
+      <c r="E939" t="s">
+        <v>1</v>
+      </c>
+      <c r="F939" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="940" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A940" t="s">
+        <v>2</v>
+      </c>
+      <c r="B940" t="s">
+        <v>11</v>
+      </c>
+      <c r="C940" t="s">
+        <v>0</v>
+      </c>
+      <c r="D940">
+        <v>4.97</v>
+      </c>
+      <c r="E940" t="s">
+        <v>1</v>
+      </c>
+      <c r="F940" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="941" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A941" t="s">
+        <v>2</v>
+      </c>
+      <c r="B941" t="s">
+        <v>11</v>
+      </c>
+      <c r="C941" t="s">
+        <v>0</v>
+      </c>
+      <c r="D941">
+        <v>5.31</v>
+      </c>
+      <c r="E941" t="s">
+        <v>1</v>
+      </c>
+      <c r="F941" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="942" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A942" t="s">
+        <v>2</v>
+      </c>
+      <c r="B942" t="s">
+        <v>11</v>
+      </c>
+      <c r="C942" t="s">
+        <v>0</v>
+      </c>
+      <c r="D942">
+        <v>6.56</v>
+      </c>
+      <c r="E942" t="s">
+        <v>1</v>
+      </c>
+      <c r="F942" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="943" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A943" t="s">
+        <v>2</v>
+      </c>
+      <c r="B943" t="s">
+        <v>11</v>
+      </c>
+      <c r="C943" t="s">
+        <v>0</v>
+      </c>
+      <c r="D943">
+        <v>11.41</v>
+      </c>
+      <c r="E943" t="s">
+        <v>1</v>
+      </c>
+      <c r="F943" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="944" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A944" t="s">
+        <v>2</v>
+      </c>
+      <c r="B944" t="s">
+        <v>11</v>
+      </c>
+      <c r="C944" t="s">
+        <v>0</v>
+      </c>
+      <c r="D944">
+        <v>9.34</v>
+      </c>
+      <c r="E944" t="s">
+        <v>1</v>
+      </c>
+      <c r="F944" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="945" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A945" t="s">
+        <v>2</v>
+      </c>
+      <c r="B945" t="s">
+        <v>11</v>
+      </c>
+      <c r="C945" t="s">
+        <v>0</v>
+      </c>
+      <c r="D945">
+        <v>13.13</v>
+      </c>
+      <c r="E945" t="s">
+        <v>1</v>
+      </c>
+      <c r="F945" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="946" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A946" t="s">
+        <v>2</v>
+      </c>
+      <c r="B946" t="s">
+        <v>11</v>
+      </c>
+      <c r="C946" t="s">
+        <v>0</v>
+      </c>
+      <c r="D946">
+        <v>6.42</v>
+      </c>
+      <c r="E946" t="s">
+        <v>1</v>
+      </c>
+      <c r="F946" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="947" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A947" t="s">
+        <v>2</v>
+      </c>
+      <c r="B947" t="s">
+        <v>11</v>
+      </c>
+      <c r="C947" t="s">
+        <v>0</v>
+      </c>
+      <c r="D947">
+        <v>5.5</v>
+      </c>
+      <c r="E947" t="s">
+        <v>1</v>
+      </c>
+      <c r="F947" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="948" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A948" t="s">
+        <v>2</v>
+      </c>
+      <c r="B948" t="s">
+        <v>11</v>
+      </c>
+      <c r="C948" t="s">
+        <v>0</v>
+      </c>
+      <c r="D948">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E948" t="s">
+        <v>1</v>
+      </c>
+      <c r="F948" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="949" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A949" t="s">
+        <v>2</v>
+      </c>
+      <c r="B949" t="s">
+        <v>11</v>
+      </c>
+      <c r="C949" t="s">
+        <v>0</v>
+      </c>
+      <c r="D949">
+        <v>3.77</v>
+      </c>
+      <c r="E949" t="s">
+        <v>1</v>
+      </c>
+      <c r="F949" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="950" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A950" t="s">
+        <v>2</v>
+      </c>
+      <c r="B950" t="s">
+        <v>11</v>
+      </c>
+      <c r="C950" t="s">
+        <v>0</v>
+      </c>
+      <c r="D950">
+        <v>2.56</v>
+      </c>
+      <c r="E950" t="s">
+        <v>1</v>
+      </c>
+      <c r="F950" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="951" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A951" t="s">
+        <v>2</v>
+      </c>
+      <c r="B951" t="s">
+        <v>11</v>
+      </c>
+      <c r="C951" t="s">
+        <v>0</v>
+      </c>
+      <c r="D951">
+        <v>2.1</v>
+      </c>
+      <c r="E951" t="s">
+        <v>1</v>
+      </c>
+      <c r="F951" s="1">
+        <v>44848</v>
+      </c>
+    </row>
+    <row r="952" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A952" t="s">
+        <v>2</v>
+      </c>
+      <c r="B952" t="s">
+        <v>11</v>
+      </c>
+      <c r="C952" t="s">
+        <v>0</v>
+      </c>
+      <c r="D952">
+        <v>5.82</v>
+      </c>
+      <c r="E952" t="s">
+        <v>1</v>
+      </c>
+      <c r="F952" s="1">
+        <v>44848</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update as of 5/10
</commit_message>
<xml_diff>
--- a/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
+++ b/Tia_Jub39/2022-08-31_cest-2.1_JUB39_SOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiabrown/Documents/git/cest-2.1-Project/Tia_Jub39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436EAADC-8BAE-C44E-AF84-A8BC61A14185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95ECBC0-3ED8-D349-A570-9A455C102E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15600" xr2:uid="{DD7AC6D9-FEFD-0E41-A755-99DADF736280}"/>
   </bookViews>
@@ -446,9 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A9CC03-DE84-E245-89A8-02F35FB81FD2}">
   <dimension ref="A1:F952"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A929" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H936" sqref="H936"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18053,7 +18051,7 @@
         <v>1</v>
       </c>
       <c r="F880" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="881" spans="1:6" x14ac:dyDescent="0.2">
@@ -18073,7 +18071,7 @@
         <v>1</v>
       </c>
       <c r="F881" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="882" spans="1:6" x14ac:dyDescent="0.2">
@@ -18093,7 +18091,7 @@
         <v>1</v>
       </c>
       <c r="F882" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="883" spans="1:6" x14ac:dyDescent="0.2">
@@ -18113,7 +18111,7 @@
         <v>1</v>
       </c>
       <c r="F883" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="884" spans="1:6" x14ac:dyDescent="0.2">
@@ -18133,7 +18131,7 @@
         <v>1</v>
       </c>
       <c r="F884" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="885" spans="1:6" x14ac:dyDescent="0.2">
@@ -18153,7 +18151,7 @@
         <v>1</v>
       </c>
       <c r="F885" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="886" spans="1:6" x14ac:dyDescent="0.2">
@@ -18173,7 +18171,7 @@
         <v>1</v>
       </c>
       <c r="F886" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="887" spans="1:6" x14ac:dyDescent="0.2">
@@ -18193,7 +18191,7 @@
         <v>1</v>
       </c>
       <c r="F887" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="888" spans="1:6" x14ac:dyDescent="0.2">
@@ -18213,7 +18211,7 @@
         <v>1</v>
       </c>
       <c r="F888" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="889" spans="1:6" x14ac:dyDescent="0.2">
@@ -18233,7 +18231,7 @@
         <v>1</v>
       </c>
       <c r="F889" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="890" spans="1:6" x14ac:dyDescent="0.2">
@@ -18253,7 +18251,7 @@
         <v>1</v>
       </c>
       <c r="F890" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="891" spans="1:6" x14ac:dyDescent="0.2">
@@ -18273,7 +18271,7 @@
         <v>1</v>
       </c>
       <c r="F891" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="892" spans="1:6" x14ac:dyDescent="0.2">
@@ -18293,7 +18291,7 @@
         <v>1</v>
       </c>
       <c r="F892" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="893" spans="1:6" x14ac:dyDescent="0.2">
@@ -18313,7 +18311,7 @@
         <v>1</v>
       </c>
       <c r="F893" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="894" spans="1:6" x14ac:dyDescent="0.2">
@@ -18333,7 +18331,7 @@
         <v>1</v>
       </c>
       <c r="F894" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="895" spans="1:6" x14ac:dyDescent="0.2">
@@ -18353,7 +18351,7 @@
         <v>1</v>
       </c>
       <c r="F895" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="896" spans="1:6" x14ac:dyDescent="0.2">
@@ -18373,7 +18371,7 @@
         <v>1</v>
       </c>
       <c r="F896" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="897" spans="1:6" x14ac:dyDescent="0.2">
@@ -18393,7 +18391,7 @@
         <v>1</v>
       </c>
       <c r="F897" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="898" spans="1:6" x14ac:dyDescent="0.2">
@@ -18413,7 +18411,7 @@
         <v>1</v>
       </c>
       <c r="F898" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="899" spans="1:6" x14ac:dyDescent="0.2">
@@ -18433,7 +18431,7 @@
         <v>1</v>
       </c>
       <c r="F899" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="900" spans="1:6" x14ac:dyDescent="0.2">
@@ -18453,7 +18451,7 @@
         <v>1</v>
       </c>
       <c r="F900" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="901" spans="1:6" x14ac:dyDescent="0.2">
@@ -18473,7 +18471,7 @@
         <v>1</v>
       </c>
       <c r="F901" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="902" spans="1:6" x14ac:dyDescent="0.2">
@@ -18493,7 +18491,7 @@
         <v>1</v>
       </c>
       <c r="F902" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="903" spans="1:6" x14ac:dyDescent="0.2">
@@ -18513,7 +18511,7 @@
         <v>1</v>
       </c>
       <c r="F903" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="904" spans="1:6" x14ac:dyDescent="0.2">
@@ -18533,7 +18531,7 @@
         <v>1</v>
       </c>
       <c r="F904" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="905" spans="1:6" x14ac:dyDescent="0.2">
@@ -18553,7 +18551,7 @@
         <v>1</v>
       </c>
       <c r="F905" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="906" spans="1:6" x14ac:dyDescent="0.2">
@@ -18573,7 +18571,7 @@
         <v>1</v>
       </c>
       <c r="F906" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="907" spans="1:6" x14ac:dyDescent="0.2">
@@ -18593,7 +18591,7 @@
         <v>1</v>
       </c>
       <c r="F907" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="908" spans="1:6" x14ac:dyDescent="0.2">
@@ -18613,7 +18611,7 @@
         <v>1</v>
       </c>
       <c r="F908" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="909" spans="1:6" x14ac:dyDescent="0.2">
@@ -18633,7 +18631,7 @@
         <v>1</v>
       </c>
       <c r="F909" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="910" spans="1:6" x14ac:dyDescent="0.2">
@@ -18653,7 +18651,7 @@
         <v>1</v>
       </c>
       <c r="F910" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="911" spans="1:6" x14ac:dyDescent="0.2">
@@ -18673,7 +18671,7 @@
         <v>1</v>
       </c>
       <c r="F911" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="912" spans="1:6" x14ac:dyDescent="0.2">
@@ -18693,7 +18691,7 @@
         <v>1</v>
       </c>
       <c r="F912" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="913" spans="1:6" x14ac:dyDescent="0.2">
@@ -18713,7 +18711,7 @@
         <v>1</v>
       </c>
       <c r="F913" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="914" spans="1:6" x14ac:dyDescent="0.2">
@@ -18733,7 +18731,7 @@
         <v>1</v>
       </c>
       <c r="F914" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="915" spans="1:6" x14ac:dyDescent="0.2">
@@ -18753,7 +18751,7 @@
         <v>1</v>
       </c>
       <c r="F915" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="916" spans="1:6" x14ac:dyDescent="0.2">
@@ -18773,7 +18771,7 @@
         <v>1</v>
       </c>
       <c r="F916" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="917" spans="1:6" x14ac:dyDescent="0.2">
@@ -18793,7 +18791,7 @@
         <v>1</v>
       </c>
       <c r="F917" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="918" spans="1:6" x14ac:dyDescent="0.2">
@@ -18813,7 +18811,7 @@
         <v>1</v>
       </c>
       <c r="F918" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="919" spans="1:6" x14ac:dyDescent="0.2">
@@ -18833,7 +18831,7 @@
         <v>1</v>
       </c>
       <c r="F919" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="920" spans="1:6" x14ac:dyDescent="0.2">
@@ -18853,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="F920" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="921" spans="1:6" x14ac:dyDescent="0.2">
@@ -18873,7 +18871,7 @@
         <v>1</v>
       </c>
       <c r="F921" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="922" spans="1:6" x14ac:dyDescent="0.2">
@@ -18893,7 +18891,7 @@
         <v>1</v>
       </c>
       <c r="F922" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="923" spans="1:6" x14ac:dyDescent="0.2">
@@ -18913,7 +18911,7 @@
         <v>1</v>
       </c>
       <c r="F923" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="924" spans="1:6" x14ac:dyDescent="0.2">
@@ -18933,7 +18931,7 @@
         <v>1</v>
       </c>
       <c r="F924" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="925" spans="1:6" x14ac:dyDescent="0.2">
@@ -18953,7 +18951,7 @@
         <v>1</v>
       </c>
       <c r="F925" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="926" spans="1:6" x14ac:dyDescent="0.2">
@@ -18973,7 +18971,7 @@
         <v>1</v>
       </c>
       <c r="F926" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="927" spans="1:6" x14ac:dyDescent="0.2">
@@ -18993,7 +18991,7 @@
         <v>1</v>
       </c>
       <c r="F927" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="928" spans="1:6" x14ac:dyDescent="0.2">
@@ -19013,7 +19011,7 @@
         <v>1</v>
       </c>
       <c r="F928" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="929" spans="1:6" x14ac:dyDescent="0.2">
@@ -19033,7 +19031,7 @@
         <v>1</v>
       </c>
       <c r="F929" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="930" spans="1:6" x14ac:dyDescent="0.2">
@@ -19053,7 +19051,7 @@
         <v>1</v>
       </c>
       <c r="F930" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="931" spans="1:6" x14ac:dyDescent="0.2">
@@ -19073,7 +19071,7 @@
         <v>1</v>
       </c>
       <c r="F931" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="932" spans="1:6" x14ac:dyDescent="0.2">
@@ -19093,7 +19091,7 @@
         <v>1</v>
       </c>
       <c r="F932" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="933" spans="1:6" x14ac:dyDescent="0.2">
@@ -19113,7 +19111,7 @@
         <v>1</v>
       </c>
       <c r="F933" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="934" spans="1:6" x14ac:dyDescent="0.2">
@@ -19133,7 +19131,7 @@
         <v>1</v>
       </c>
       <c r="F934" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="935" spans="1:6" x14ac:dyDescent="0.2">
@@ -19153,7 +19151,7 @@
         <v>1</v>
       </c>
       <c r="F935" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="936" spans="1:6" x14ac:dyDescent="0.2">
@@ -19173,7 +19171,7 @@
         <v>1</v>
       </c>
       <c r="F936" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="937" spans="1:6" x14ac:dyDescent="0.2">
@@ -19193,7 +19191,7 @@
         <v>1</v>
       </c>
       <c r="F937" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="938" spans="1:6" x14ac:dyDescent="0.2">
@@ -19213,7 +19211,7 @@
         <v>1</v>
       </c>
       <c r="F938" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="939" spans="1:6" x14ac:dyDescent="0.2">
@@ -19233,7 +19231,7 @@
         <v>1</v>
       </c>
       <c r="F939" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="940" spans="1:6" x14ac:dyDescent="0.2">
@@ -19253,7 +19251,7 @@
         <v>1</v>
       </c>
       <c r="F940" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="941" spans="1:6" x14ac:dyDescent="0.2">
@@ -19273,7 +19271,7 @@
         <v>1</v>
       </c>
       <c r="F941" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="942" spans="1:6" x14ac:dyDescent="0.2">
@@ -19293,7 +19291,7 @@
         <v>1</v>
       </c>
       <c r="F942" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="943" spans="1:6" x14ac:dyDescent="0.2">
@@ -19313,7 +19311,7 @@
         <v>1</v>
       </c>
       <c r="F943" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="944" spans="1:6" x14ac:dyDescent="0.2">
@@ -19333,7 +19331,7 @@
         <v>1</v>
       </c>
       <c r="F944" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="945" spans="1:6" x14ac:dyDescent="0.2">
@@ -19353,7 +19351,7 @@
         <v>1</v>
       </c>
       <c r="F945" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="946" spans="1:6" x14ac:dyDescent="0.2">
@@ -19373,7 +19371,7 @@
         <v>1</v>
       </c>
       <c r="F946" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="947" spans="1:6" x14ac:dyDescent="0.2">
@@ -19393,7 +19391,7 @@
         <v>1</v>
       </c>
       <c r="F947" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="948" spans="1:6" x14ac:dyDescent="0.2">
@@ -19413,7 +19411,7 @@
         <v>1</v>
       </c>
       <c r="F948" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="949" spans="1:6" x14ac:dyDescent="0.2">
@@ -19433,7 +19431,7 @@
         <v>1</v>
       </c>
       <c r="F949" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="950" spans="1:6" x14ac:dyDescent="0.2">
@@ -19453,7 +19451,7 @@
         <v>1</v>
       </c>
       <c r="F950" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="951" spans="1:6" x14ac:dyDescent="0.2">
@@ -19473,7 +19471,7 @@
         <v>1</v>
       </c>
       <c r="F951" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
     <row r="952" spans="1:6" x14ac:dyDescent="0.2">
@@ -19493,7 +19491,7 @@
         <v>1</v>
       </c>
       <c r="F952" s="1">
-        <v>44848</v>
+        <v>44847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>